<commit_message>
Added excel file for tables creation; improved main thesis doc; and added new schema on ppt file.
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -4,12 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26640" yWindow="180" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="26800" yWindow="240" windowWidth="25600" windowHeight="15420" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="118">
   <si>
     <t>ACCESSIBILITY</t>
   </si>
@@ -268,12 +273,228 @@
   <si>
     <t>Confidentiality</t>
   </si>
+  <si>
+    <t>SERVICE QUALITY</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Response Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kritikos et al. (2013) </t>
+  </si>
+  <si>
+    <t>Zeithaml et al. (2001)</t>
+  </si>
+  <si>
+    <t>Cox and Dale (2001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yang et al. (2003) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parasuraman et al. (2005) </t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Ease of navigation</t>
+  </si>
+  <si>
+    <t>Security/Privacy</t>
+  </si>
+  <si>
+    <t>Ease of navigation; Site aesthetics</t>
+  </si>
+  <si>
+    <t>Ease of use; Aesthetic design</t>
+  </si>
+  <si>
+    <t>Website appearance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raman et al. (2008) </t>
+  </si>
+  <si>
+    <t>Appearance; Ease of use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yoo and Donthu (2001) </t>
+  </si>
+  <si>
+    <t>Processing speed</t>
+  </si>
+  <si>
+    <t>Wolfinbarger and Gilly (2003)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lociacono et al. (2002) </t>
+  </si>
+  <si>
+    <t>Response time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bressolles (2008) </t>
+  </si>
+  <si>
+    <t>Security/privacy</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>E-S-QUAL</t>
+  </si>
+  <si>
+    <t>WebQual</t>
+  </si>
+  <si>
+    <t>Trust</t>
+  </si>
+  <si>
+    <t>Design; Intuitiveness; Visual appeal</t>
+  </si>
+  <si>
+    <t>WebQual 4</t>
+  </si>
+  <si>
+    <t>e-TailQ</t>
+  </si>
+  <si>
+    <t>Website design</t>
+  </si>
+  <si>
+    <t>Fulfillment/Reliability</t>
+  </si>
+  <si>
+    <t>SITEQUAL</t>
+  </si>
+  <si>
+    <t>NetQual</t>
+  </si>
+  <si>
+    <t>Ease of use; Site design</t>
+  </si>
+  <si>
+    <t>Visual appeal</t>
+  </si>
+  <si>
+    <t>Visual appeal; Intuitiveness</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>Ease of Use</t>
+  </si>
+  <si>
+    <t>Time Behavior</t>
+  </si>
+  <si>
+    <t>Aesthetic design</t>
+  </si>
+  <si>
+    <t>Interactive responsiveness</t>
+  </si>
+  <si>
+    <t>Site aesthetics</t>
+  </si>
+  <si>
+    <t>Understanding</t>
+  </si>
+  <si>
+    <t>Prompt delivery</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>Competence</t>
+  </si>
+  <si>
+    <t>Reliability</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Fulfillment</t>
+  </si>
+  <si>
+    <t>Appearance</t>
+  </si>
+  <si>
+    <t>Reliability/fulfillment</t>
+  </si>
+  <si>
+    <t>Site design</t>
+  </si>
+  <si>
+    <t>Functional completeness &amp; Functional correctness</t>
+  </si>
+  <si>
+    <t>ISO/IEC 25010:2011 (Product Quality)</t>
+  </si>
+  <si>
+    <t>e-service quality dimensions</t>
+  </si>
+  <si>
+    <t>Product quality characteristic</t>
+  </si>
+  <si>
+    <t>Quality in use characteristic</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>Perceived by user</t>
+  </si>
+  <si>
+    <t>Provided in product</t>
+  </si>
+  <si>
+    <t>Hypethesis</t>
+  </si>
+  <si>
+    <t>Qualitative characteristics (Convenience, Performance, Trustworthiness, Compatibility)</t>
+  </si>
+  <si>
+    <t>Qualitative characteristics (Compatibility, Functionality, Reliability)</t>
+  </si>
+  <si>
+    <t>Software properties</t>
+  </si>
+  <si>
+    <t>Inherent characteristics</t>
+  </si>
+  <si>
+    <t>Assigned characteristics</t>
+  </si>
+  <si>
+    <t>Inspired on figure C.6 - Software properties</t>
+  </si>
+  <si>
+    <t>Document: BS-ISO-IEC 25010:2011</t>
+  </si>
+  <si>
+    <t>Security / Privacy</t>
+  </si>
+  <si>
+    <t>e-service AUES dimentional components</t>
+  </si>
+  <si>
+    <t>e-service Quality dimensions (AUES)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -306,6 +527,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -314,6 +542,24 @@
       <sz val="7"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -336,7 +582,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -415,6 +661,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -432,6 +689,26 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -535,7 +812,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -585,24 +862,206 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -619,6 +1078,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -630,10 +1092,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -645,35 +1107,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -682,8 +1150,213 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="201">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -708,6 +1381,82 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -732,6 +1481,82 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1079,114 +1904,114 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="21" customHeight="1">
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17"/>
-    </row>
-    <row r="3" spans="2:9" s="12" customFormat="1" ht="20" customHeight="1">
-      <c r="B3" s="18"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="19" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
+    </row>
+    <row r="3" spans="2:9" s="23" customFormat="1" ht="20" customHeight="1">
+      <c r="B3" s="29"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:9" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="B4" s="20" t="s">
+    <row r="4" spans="2:9" s="13" customFormat="1" ht="21" customHeight="1">
+      <c r="B4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="2:9" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="B5" s="20"/>
-      <c r="C5" s="22" t="s">
+      <c r="D4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="2:9" s="13" customFormat="1" ht="21" customHeight="1">
+      <c r="B5" s="31"/>
+      <c r="C5" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="2:9" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="B6" s="20"/>
-      <c r="C6" s="23" t="s">
+      <c r="D5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="2:9" s="13" customFormat="1" ht="21" customHeight="1">
+      <c r="B6" s="31"/>
+      <c r="C6" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="2:9" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="B7" s="20"/>
-      <c r="C7" s="24" t="s">
+      <c r="D6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="2:9" s="13" customFormat="1" ht="21" customHeight="1">
+      <c r="B7" s="31"/>
+      <c r="C7" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="11" t="s">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1221,90 +2046,90 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" thickBot="1">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="36"/>
+      <c r="B3" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="25"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" ht="26" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="25"/>
-      <c r="B4" s="28" t="s">
+      <c r="A4" s="36"/>
+      <c r="B4" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="36"/>
     </row>
     <row r="5" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A5" s="25"/>
-      <c r="B5" s="28" t="s">
+      <c r="A5" s="36"/>
+      <c r="B5" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A6" s="25"/>
-      <c r="B6" s="28" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="25"/>
+      <c r="D6" s="36"/>
     </row>
     <row r="7" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A7" s="25"/>
-      <c r="B7" s="28" t="s">
+      <c r="A7" s="36"/>
+      <c r="B7" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="25"/>
+      <c r="D7" s="36"/>
     </row>
     <row r="8" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A8" s="25"/>
-      <c r="B8" s="28" t="s">
+      <c r="A8" s="36"/>
+      <c r="B8" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="36"/>
     </row>
     <row r="9" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="29" t="s">
+      <c r="A9" s="36"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="25"/>
+      <c r="D9" s="36"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1319,152 +2144,650 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:J22"/>
+  <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="1.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:10">
-      <c r="F5" s="2" t="s">
+    <row r="2" spans="2:10">
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="F7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="2:10" ht="45" customHeight="1">
-      <c r="B6" s="31" t="s">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="2:10" s="2" customFormat="1" ht="45" customHeight="1">
+      <c r="B8" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31" t="s">
+      <c r="C8" s="44"/>
+      <c r="D8" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E8" s="44" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="D7" s="32" t="s">
+      <c r="F8" s="46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="D9" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="D8" s="32"/>
-      <c r="E8" s="1" t="s">
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="D10" s="45"/>
+      <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
-      <c r="D9" s="32"/>
-      <c r="E9" s="1" t="s">
+    <row r="11" spans="2:10">
+      <c r="D11" s="45"/>
+      <c r="E11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="D10" s="32" t="s">
+    <row r="12" spans="2:10">
+      <c r="D12" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="D11" s="32"/>
-      <c r="E11" s="1" t="s">
+    <row r="13" spans="2:10">
+      <c r="D13" s="45"/>
+      <c r="E13" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
-      <c r="D12" s="32"/>
-      <c r="E12" s="1" t="s">
+    <row r="14" spans="2:10">
+      <c r="D14" s="45"/>
+      <c r="E14" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
-      <c r="D13" s="32" t="s">
+    <row r="15" spans="2:10">
+      <c r="D15" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
-      <c r="D14" s="32"/>
-      <c r="E14" s="1" t="s">
+    <row r="16" spans="2:10">
+      <c r="D16" s="45"/>
+      <c r="E16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
-      <c r="D15" s="32"/>
-      <c r="E15" s="1" t="s">
+    <row r="17" spans="4:6">
+      <c r="D17" s="45"/>
+      <c r="E17" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
-      <c r="D16" s="32"/>
-      <c r="E16" s="1" t="s">
+    <row r="18" spans="4:6">
+      <c r="D18" s="45"/>
+      <c r="E18" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="4:5">
-      <c r="D17" s="32"/>
-      <c r="E17" s="1" t="s">
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6">
+      <c r="D19" s="45"/>
+      <c r="E19" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="4:5">
-      <c r="D18" s="32" t="s">
+    <row r="20" spans="4:6">
+      <c r="D20" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="4:5">
-      <c r="D19" s="32"/>
-      <c r="E19" s="1" t="s">
+    <row r="21" spans="4:6">
+      <c r="D21" s="45"/>
+      <c r="E21" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="4:5">
-      <c r="D20" s="32"/>
-      <c r="E20" s="1" t="s">
+    <row r="22" spans="4:6">
+      <c r="D22" s="45"/>
+      <c r="E22" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="4:5">
-      <c r="D21" s="32"/>
-      <c r="E21" s="1" t="s">
+    <row r="23" spans="4:6">
+      <c r="D23" s="45"/>
+      <c r="E23" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="4:5">
-      <c r="D22" s="32"/>
-      <c r="E22" s="1" t="s">
+    <row r="24" spans="4:6">
+      <c r="D24" s="45"/>
+      <c r="E24" s="2" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="D18:D22"/>
+  <mergeCells count="6">
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H23"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="1.83203125" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" customWidth="1"/>
+    <col min="9" max="9" width="26.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8">
+      <c r="B2" s="38"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+    </row>
+    <row r="3" spans="2:8" ht="24" customHeight="1">
+      <c r="B3" s="36"/>
+      <c r="C3" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="36"/>
+    </row>
+    <row r="4" spans="2:8" ht="27" customHeight="1">
+      <c r="B4" s="38"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="109" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="36"/>
+    </row>
+    <row r="5" spans="2:8" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="B5" s="37"/>
+      <c r="C5" s="111" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="112" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="113" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="113" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="114" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="37"/>
+    </row>
+    <row r="6" spans="2:8" ht="20" customHeight="1">
+      <c r="B6" s="38"/>
+      <c r="C6" s="78" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="36"/>
+    </row>
+    <row r="7" spans="2:8" ht="20" customHeight="1">
+      <c r="B7" s="38"/>
+      <c r="C7" s="95" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="36"/>
+    </row>
+    <row r="8" spans="2:8" ht="20" customHeight="1">
+      <c r="B8" s="36"/>
+      <c r="C8" s="110" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="36"/>
+    </row>
+    <row r="9" spans="2:8" ht="20" customHeight="1">
+      <c r="B9" s="36"/>
+      <c r="C9" s="95" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="36"/>
+    </row>
+    <row r="10" spans="2:8" ht="20" customHeight="1">
+      <c r="B10" s="36"/>
+      <c r="C10" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="36"/>
+    </row>
+    <row r="11" spans="2:8" ht="20" customHeight="1">
+      <c r="B11" s="36"/>
+      <c r="C11" s="95" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="36"/>
+    </row>
+    <row r="12" spans="2:8" ht="20" customHeight="1">
+      <c r="B12" s="36"/>
+      <c r="C12" s="110" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="36"/>
+    </row>
+    <row r="13" spans="2:8" ht="20" customHeight="1">
+      <c r="B13" s="36"/>
+      <c r="C13" s="95" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="36"/>
+    </row>
+    <row r="14" spans="2:8" ht="23" customHeight="1">
+      <c r="B14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="36"/>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="C15" s="46"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22" s="48"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="C23" s="48"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="C3:C4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="36"/>
+      <c r="B3" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="36"/>
+    </row>
+    <row r="4" spans="1:7" ht="25" customHeight="1">
+      <c r="A4" s="36"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="36"/>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A5" s="37"/>
+      <c r="B5" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="65"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="68"/>
+      <c r="G5" s="37"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A6" s="37"/>
+      <c r="B6" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="57"/>
+      <c r="D6" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="37"/>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A7" s="37"/>
+      <c r="B7" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="50"/>
+      <c r="D7" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="71"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="37"/>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A8" s="37"/>
+      <c r="B8" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="37"/>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A9" s="37"/>
+      <c r="B9" s="72" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="50"/>
+      <c r="D9" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="37"/>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A10" s="37"/>
+      <c r="B10" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="61"/>
+      <c r="D10" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="64" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="37"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1473,4 +2796,737 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" customWidth="1"/>
+    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.5" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+    </row>
+    <row r="2" spans="1:15" ht="22" customHeight="1">
+      <c r="A2" s="36"/>
+      <c r="B2" s="83" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="23"/>
+    </row>
+    <row r="3" spans="1:15" ht="39" customHeight="1">
+      <c r="A3" s="36"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="80" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="80" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="76" t="s">
+        <v>100</v>
+      </c>
+      <c r="M3" s="38"/>
+    </row>
+    <row r="4" spans="1:15" ht="30" customHeight="1">
+      <c r="A4" s="36"/>
+      <c r="B4" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="96"/>
+      <c r="D4" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="98" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="36"/>
+    </row>
+    <row r="5" spans="1:15" ht="30" customHeight="1">
+      <c r="A5" s="36"/>
+      <c r="B5" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="84"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="36"/>
+    </row>
+    <row r="6" spans="1:15" ht="30" customHeight="1">
+      <c r="A6" s="36"/>
+      <c r="B6" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="101"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="102" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="102"/>
+      <c r="I6" s="102" t="s">
+        <v>94</v>
+      </c>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="104" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="36"/>
+    </row>
+    <row r="7" spans="1:15" ht="30">
+      <c r="A7" s="36"/>
+      <c r="B7" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="85"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="90"/>
+      <c r="M7" s="36"/>
+    </row>
+    <row r="8" spans="1:15" ht="30" customHeight="1">
+      <c r="A8" s="36"/>
+      <c r="B8" s="95" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="101"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="103"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="104" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="36"/>
+    </row>
+    <row r="9" spans="1:15" ht="30">
+      <c r="A9" s="36"/>
+      <c r="B9" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="85" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" s="85" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="36"/>
+    </row>
+    <row r="10" spans="1:15" ht="30" customHeight="1">
+      <c r="A10" s="36"/>
+      <c r="B10" s="95" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="101"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="102" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="102"/>
+      <c r="J10" s="102" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="102"/>
+      <c r="L10" s="104" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="36"/>
+    </row>
+    <row r="11" spans="1:15" ht="30">
+      <c r="A11" s="36"/>
+      <c r="B11" s="78" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="84" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="85"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="36"/>
+    </row>
+    <row r="12" spans="1:15" ht="30" customHeight="1">
+      <c r="A12" s="36"/>
+      <c r="B12" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="101"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="105" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="102"/>
+      <c r="J12" s="102"/>
+      <c r="K12" s="102"/>
+      <c r="L12" s="106"/>
+      <c r="M12" s="36"/>
+    </row>
+    <row r="13" spans="1:15" ht="30">
+      <c r="A13" s="36"/>
+      <c r="B13" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="85" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85"/>
+      <c r="L13" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="36"/>
+    </row>
+    <row r="14" spans="1:15" ht="37" customHeight="1">
+      <c r="A14" s="36"/>
+      <c r="B14" s="95" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="101"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="102" t="s">
+        <v>95</v>
+      </c>
+      <c r="J14" s="102"/>
+      <c r="K14" s="102" t="s">
+        <v>97</v>
+      </c>
+      <c r="L14" s="107" t="s">
+        <v>99</v>
+      </c>
+      <c r="M14" s="36"/>
+    </row>
+    <row r="15" spans="1:15" ht="30" customHeight="1">
+      <c r="A15" s="36"/>
+      <c r="B15" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="84"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="100"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="85"/>
+      <c r="L15" s="91"/>
+      <c r="M15" s="36"/>
+      <c r="O15" s="23"/>
+    </row>
+    <row r="16" spans="1:15" ht="30" customHeight="1">
+      <c r="A16" s="36"/>
+      <c r="B16" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="101"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="103"/>
+      <c r="L16" s="104" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="36"/>
+      <c r="O16" s="23"/>
+    </row>
+    <row r="17" spans="1:15" ht="30">
+      <c r="A17" s="36"/>
+      <c r="B17" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="84"/>
+      <c r="D17" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="85"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="100"/>
+      <c r="I17" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="85"/>
+      <c r="K17" s="100" t="s">
+        <v>115</v>
+      </c>
+      <c r="L17" s="91"/>
+      <c r="M17" s="36"/>
+      <c r="O17" s="23"/>
+    </row>
+    <row r="18" spans="1:15" ht="30" customHeight="1">
+      <c r="A18" s="36"/>
+      <c r="B18" s="95" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="101"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="103"/>
+      <c r="I18" s="102"/>
+      <c r="J18" s="102"/>
+      <c r="K18" s="103"/>
+      <c r="L18" s="104" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="36"/>
+      <c r="O18" s="23"/>
+    </row>
+    <row r="19" spans="1:15" ht="30" customHeight="1">
+      <c r="A19" s="36"/>
+      <c r="B19" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="92"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="108"/>
+      <c r="L19" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="36"/>
+      <c r="O19" s="23"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="B2:B3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B7:N15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="2:14">
+      <c r="D7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="2:14" ht="28" customHeight="1">
+      <c r="D8" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="2:14" ht="18">
+      <c r="B9" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="H9" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="75"/>
+    </row>
+    <row r="10" spans="2:14" ht="18">
+      <c r="B10" s="47"/>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="75"/>
+    </row>
+    <row r="11" spans="2:14" ht="18">
+      <c r="B11" s="47"/>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="75"/>
+    </row>
+    <row r="12" spans="2:14" ht="18">
+      <c r="B12" s="47"/>
+      <c r="C12" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="75"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="75"/>
+    </row>
+    <row r="13" spans="2:14" ht="18">
+      <c r="B13" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="45"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="75"/>
+      <c r="H13" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="45"/>
+      <c r="J13" s="75"/>
+    </row>
+    <row r="14" spans="2:14" ht="18">
+      <c r="B14" s="47"/>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="75"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="75"/>
+    </row>
+    <row r="15" spans="2:14" ht="18">
+      <c r="B15" s="47"/>
+      <c r="C15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="75"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" s="75"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="H13:H15"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:5" ht="114" customHeight="1">
+      <c r="C5" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="80" customHeight="1">
+      <c r="C6" s="77"/>
+      <c r="D6" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="76" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5">
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5">
+      <c r="C9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C5:C6"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated main document, updated model in pptx, and tables.
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -9,12 +9,11 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId7"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="111">
   <si>
     <t>ACCESSIBILITY</t>
   </si>
@@ -214,18 +213,9 @@
     </r>
   </si>
   <si>
-    <t>e-service Qualitative characteristic</t>
-  </si>
-  <si>
-    <t>e-service Quality dimension</t>
-  </si>
-  <si>
     <t>Approach Reference</t>
   </si>
   <si>
-    <t>Key dimensional component</t>
-  </si>
-  <si>
     <t>Availability</t>
   </si>
   <si>
@@ -253,9 +243,6 @@
     <t>Customer Service</t>
   </si>
   <si>
-    <t>Time Behaviour</t>
-  </si>
-  <si>
     <t>Transaction Capability</t>
   </si>
   <si>
@@ -274,16 +261,7 @@
     <t>Confidentiality</t>
   </si>
   <si>
-    <t>SERVICE QUALITY</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
     <t>Response Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kritikos et al. (2013) </t>
   </si>
   <si>
     <t>Zeithaml et al. (2001)</t>
@@ -1015,7 +993,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1035,12 +1013,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1262,80 +1234,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1355,6 +1255,43 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="201">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1904,114 +1841,114 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="21" customHeight="1">
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28"/>
-    </row>
-    <row r="3" spans="2:9" s="23" customFormat="1" ht="20" customHeight="1">
-      <c r="B3" s="29"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="30" t="s">
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
+    </row>
+    <row r="3" spans="2:9" s="21" customFormat="1" ht="20" customHeight="1">
+      <c r="B3" s="27"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:9" s="13" customFormat="1" ht="21" customHeight="1">
-      <c r="B4" s="31" t="s">
+    <row r="4" spans="2:9" s="11" customFormat="1" ht="21" customHeight="1">
+      <c r="B4" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="2:9" s="13" customFormat="1" ht="21" customHeight="1">
-      <c r="B5" s="31"/>
-      <c r="C5" s="33" t="s">
+      <c r="D4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="2:9" s="11" customFormat="1" ht="21" customHeight="1">
+      <c r="B5" s="29"/>
+      <c r="C5" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="2:9" s="13" customFormat="1" ht="21" customHeight="1">
-      <c r="B6" s="31"/>
-      <c r="C6" s="34" t="s">
+      <c r="D5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="2:9" s="11" customFormat="1" ht="21" customHeight="1">
+      <c r="B6" s="29"/>
+      <c r="C6" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="19"/>
-    </row>
-    <row r="7" spans="2:9" s="13" customFormat="1" ht="21" customHeight="1">
-      <c r="B7" s="31"/>
-      <c r="C7" s="35" t="s">
+      <c r="D6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="2:9" s="11" customFormat="1" ht="21" customHeight="1">
+      <c r="B7" s="29"/>
+      <c r="C7" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2046,90 +1983,90 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" thickBot="1">
-      <c r="A3" s="36"/>
-      <c r="B3" s="39" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="34"/>
     </row>
     <row r="4" spans="1:4" ht="26" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="36"/>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="34"/>
     </row>
     <row r="5" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A5" s="36"/>
-      <c r="B5" s="41" t="s">
+      <c r="A5" s="34"/>
+      <c r="B5" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="34"/>
     </row>
     <row r="6" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="41" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A7" s="36"/>
-      <c r="B7" s="41" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="36"/>
+      <c r="D7" s="34"/>
     </row>
     <row r="8" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A8" s="36"/>
-      <c r="B8" s="41" t="s">
+      <c r="A8" s="34"/>
+      <c r="B8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="36"/>
+      <c r="D8" s="34"/>
     </row>
     <row r="9" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A9" s="36"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="42" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="36"/>
+      <c r="D9" s="34"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2144,200 +2081,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="1.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:10">
-      <c r="B2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="2:10">
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="F7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="2:10" s="2" customFormat="1" ht="45" customHeight="1">
-      <c r="B8" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="46" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="D9" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="D10" s="45"/>
-      <c r="E10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="D11" s="45"/>
-      <c r="E11" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="D12" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="D13" s="45"/>
-      <c r="E13" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="D14" s="45"/>
-      <c r="E14" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="D15" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="D16" s="45"/>
-      <c r="E16" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6">
-      <c r="D17" s="45"/>
-      <c r="E17" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6">
-      <c r="D18" s="45"/>
-      <c r="E18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6">
-      <c r="D19" s="45"/>
-      <c r="E19" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6">
-      <c r="D20" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6">
-      <c r="D21" s="45"/>
-      <c r="E21" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="4:6">
-      <c r="D22" s="45"/>
-      <c r="E22" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6">
-      <c r="D23" s="45"/>
-      <c r="E23" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6">
-      <c r="D24" s="45"/>
-      <c r="E24" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="B2:E2"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H23"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2354,198 +2101,198 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="38"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="2:8" ht="24" customHeight="1">
-      <c r="B3" s="36"/>
-      <c r="C3" s="79" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="36"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="2:8" ht="27" customHeight="1">
-      <c r="B4" s="38"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="109" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="78" t="s">
+      <c r="E4" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="78" t="s">
+      <c r="G4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="36"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="2:8" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="B5" s="37"/>
-      <c r="C5" s="111" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="85" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="86" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="112" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="113" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="113" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="114" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="37"/>
+      <c r="F5" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="2:8" ht="20" customHeight="1">
-      <c r="B6" s="38"/>
-      <c r="C6" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="90" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="90"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="2:8" ht="20" customHeight="1">
-      <c r="B7" s="38"/>
-      <c r="C7" s="95" t="s">
-        <v>62</v>
+      <c r="B7" s="36"/>
+      <c r="C7" s="82" t="s">
+        <v>55</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="34"/>
+    </row>
+    <row r="8" spans="2:8" ht="20" customHeight="1">
+      <c r="B8" s="34"/>
+      <c r="C8" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="36"/>
-    </row>
-    <row r="8" spans="2:8" ht="20" customHeight="1">
-      <c r="B8" s="36"/>
-      <c r="C8" s="110" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="36"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="90" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="90" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="91"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="2:8" ht="20" customHeight="1">
-      <c r="B9" s="36"/>
-      <c r="C9" s="95" t="s">
-        <v>52</v>
+      <c r="B9" s="34"/>
+      <c r="C9" s="82" t="s">
+        <v>45</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="36"/>
+      <c r="H9" s="34"/>
     </row>
     <row r="10" spans="2:8" ht="20" customHeight="1">
-      <c r="B10" s="36"/>
-      <c r="C10" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="36"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="76" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="89"/>
+      <c r="E10" s="90" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="2:8" ht="20" customHeight="1">
-      <c r="B11" s="36"/>
-      <c r="C11" s="95" t="s">
-        <v>53</v>
+      <c r="B11" s="34"/>
+      <c r="C11" s="82" t="s">
+        <v>46</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="36"/>
+        <v>39</v>
+      </c>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="2:8" ht="20" customHeight="1">
-      <c r="B12" s="36"/>
-      <c r="C12" s="110" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="36"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="89"/>
+      <c r="E12" s="90" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="90"/>
+      <c r="G12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="2:8" ht="20" customHeight="1">
-      <c r="B13" s="36"/>
-      <c r="C13" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="36"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="82" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="2:8" ht="23" customHeight="1">
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="36"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="2:8">
-      <c r="C15" s="46"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -2588,14 +2335,14 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="3:7">
-      <c r="C22" s="48"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="3:7">
-      <c r="C23" s="48"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2616,11 +2363,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2634,155 +2381,155 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="36"/>
-      <c r="B3" s="53" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="34"/>
+    </row>
+    <row r="4" spans="1:7" ht="25" customHeight="1">
+      <c r="A4" s="34"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="34"/>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A5" s="35"/>
+      <c r="B5" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="63"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="66"/>
+      <c r="G5" s="35"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A6" s="35"/>
+      <c r="B6" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="35"/>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A7" s="35"/>
+      <c r="B7" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="48"/>
+      <c r="D7" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="69"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="35"/>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A8" s="35"/>
+      <c r="B8" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="55"/>
+      <c r="D8" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="54" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="36"/>
-    </row>
-    <row r="4" spans="1:7" ht="25" customHeight="1">
-      <c r="A4" s="36"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="55" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="36"/>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A5" s="37"/>
-      <c r="B5" s="49" t="s">
+      <c r="E8" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="37"/>
-    </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A6" s="37"/>
-      <c r="B6" s="56" t="s">
+      <c r="F8" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="35"/>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A9" s="35"/>
+      <c r="B9" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="58" t="s">
+      <c r="C9" s="48"/>
+      <c r="D9" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="35"/>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A10" s="35"/>
+      <c r="B10" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="37"/>
-    </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A7" s="37"/>
-      <c r="B7" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="70" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="37"/>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="37"/>
-      <c r="B8" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="58" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="37"/>
-    </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A9" s="37"/>
-      <c r="B9" s="72" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="37"/>
-    </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A10" s="37"/>
-      <c r="B10" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="37"/>
+      <c r="E10" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="35"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2798,12 +2545,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2825,451 +2572,452 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="36"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="1:15" ht="22" customHeight="1">
-      <c r="A2" s="36"/>
-      <c r="B2" s="83" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="22" t="s">
+      <c r="A2" s="34"/>
+      <c r="B2" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="21"/>
+    </row>
+    <row r="3" spans="1:15" ht="39" customHeight="1">
+      <c r="A3" s="34"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="78" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="M3" s="36"/>
+    </row>
+    <row r="4" spans="1:15" ht="30" customHeight="1">
+      <c r="A4" s="34"/>
+      <c r="B4" s="82" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="34"/>
+    </row>
+    <row r="5" spans="1:15" ht="30" customHeight="1">
+      <c r="A5" s="34"/>
+      <c r="B5" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="23"/>
-    </row>
-    <row r="3" spans="1:15" ht="39" customHeight="1">
-      <c r="A3" s="36"/>
-      <c r="B3" s="83"/>
-      <c r="C3" s="82" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="80" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="76" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="76" t="s">
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="34"/>
+    </row>
+    <row r="6" spans="1:15" ht="30" customHeight="1">
+      <c r="A6" s="34"/>
+      <c r="B6" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="92" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="34"/>
+    </row>
+    <row r="7" spans="1:15" ht="30">
+      <c r="A7" s="34"/>
+      <c r="B7" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="94"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="99"/>
+      <c r="M7" s="34"/>
+    </row>
+    <row r="8" spans="1:15" ht="30" customHeight="1">
+      <c r="A8" s="34"/>
+      <c r="B8" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="92"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="92" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="96"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="34"/>
+    </row>
+    <row r="9" spans="1:15" ht="30">
+      <c r="A9" s="34"/>
+      <c r="B9" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="94" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="94" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="76" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="81" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="76" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="80" t="s">
-        <v>67</v>
-      </c>
-      <c r="L3" s="76" t="s">
-        <v>100</v>
-      </c>
-      <c r="M3" s="38"/>
-    </row>
-    <row r="4" spans="1:15" ht="30" customHeight="1">
-      <c r="A4" s="36"/>
-      <c r="B4" s="95" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="97" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="98" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97" t="s">
+      <c r="F9" s="94" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="94"/>
+      <c r="H9" s="94" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="94"/>
+      <c r="J9" s="94" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="99" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="36"/>
-    </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1">
-      <c r="A5" s="36"/>
-      <c r="B5" s="78" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="84"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="86" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="36"/>
-    </row>
-    <row r="6" spans="1:15" ht="30" customHeight="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="95" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="101"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="102" t="s">
+      <c r="L9" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="34"/>
+    </row>
+    <row r="10" spans="1:15" ht="30" customHeight="1">
+      <c r="A10" s="34"/>
+      <c r="B10" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="92"/>
+      <c r="H10" s="92" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="92"/>
+      <c r="J10" s="92" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="92"/>
+      <c r="L10" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="34"/>
+    </row>
+    <row r="11" spans="1:15" ht="30">
+      <c r="A11" s="34"/>
+      <c r="B11" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="94"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="99"/>
+      <c r="M11" s="34"/>
+    </row>
+    <row r="12" spans="1:15" ht="30" customHeight="1">
+      <c r="A12" s="34"/>
+      <c r="B12" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="92"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="100"/>
+      <c r="M12" s="34"/>
+    </row>
+    <row r="13" spans="1:15" ht="30">
+      <c r="A13" s="34"/>
+      <c r="B13" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="94" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="94" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="94"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="94"/>
+      <c r="K13" s="94"/>
+      <c r="L13" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="34"/>
+    </row>
+    <row r="14" spans="1:15" ht="37" customHeight="1">
+      <c r="A14" s="34"/>
+      <c r="B14" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" s="92"/>
+      <c r="K14" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="L14" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102" t="s">
-        <v>94</v>
-      </c>
-      <c r="J6" s="102"/>
-      <c r="K6" s="102"/>
-      <c r="L6" s="104" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="36"/>
-    </row>
-    <row r="7" spans="1:15" ht="30">
-      <c r="A7" s="36"/>
-      <c r="B7" s="78" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="85"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="88" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="89"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="88" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="88" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="90"/>
-      <c r="M7" s="36"/>
-    </row>
-    <row r="8" spans="1:15" ht="30" customHeight="1">
-      <c r="A8" s="36"/>
-      <c r="B8" s="95" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="103"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="104" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="36"/>
-    </row>
-    <row r="9" spans="1:15" ht="30">
-      <c r="A9" s="36"/>
-      <c r="B9" s="78" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="84" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="85" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" s="85" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="85" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="K9" s="85" t="s">
-        <v>98</v>
-      </c>
-      <c r="L9" s="86" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="36"/>
-    </row>
-    <row r="10" spans="1:15" ht="30" customHeight="1">
-      <c r="A10" s="36"/>
-      <c r="B10" s="95" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="101"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="102" t="s">
-        <v>93</v>
-      </c>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102" t="s">
-        <v>93</v>
-      </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="104" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="36"/>
-    </row>
-    <row r="11" spans="1:15" ht="30">
-      <c r="A11" s="36"/>
-      <c r="B11" s="78" t="s">
+      <c r="M14" s="34"/>
+    </row>
+    <row r="15" spans="1:15" ht="30" customHeight="1">
+      <c r="A15" s="34"/>
+      <c r="B15" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="84" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="88" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="85"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="36"/>
-    </row>
-    <row r="12" spans="1:15" ht="30" customHeight="1">
-      <c r="A12" s="36"/>
-      <c r="B12" s="95" t="s">
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="101"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="34"/>
+      <c r="O15" s="21"/>
+    </row>
+    <row r="16" spans="1:15" ht="30" customHeight="1">
+      <c r="A16" s="34"/>
+      <c r="B16" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="101"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="102"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="105" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="102"/>
-      <c r="J12" s="102"/>
-      <c r="K12" s="102"/>
-      <c r="L12" s="106"/>
-      <c r="M12" s="36"/>
-    </row>
-    <row r="13" spans="1:15" ht="30">
-      <c r="A13" s="36"/>
-      <c r="B13" s="78" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="84" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="85" t="s">
-        <v>66</v>
-      </c>
-      <c r="G13" s="85" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="85"/>
-      <c r="K13" s="85"/>
-      <c r="L13" s="86" t="s">
-        <v>10</v>
-      </c>
-      <c r="M13" s="36"/>
-    </row>
-    <row r="14" spans="1:15" ht="37" customHeight="1">
-      <c r="A14" s="36"/>
-      <c r="B14" s="95" t="s">
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="96"/>
+      <c r="L16" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="34"/>
+      <c r="O16" s="21"/>
+    </row>
+    <row r="17" spans="1:15" ht="30">
+      <c r="A17" s="34"/>
+      <c r="B17" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="94"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="98"/>
+      <c r="I17" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="94"/>
+      <c r="K17" s="98" t="s">
+        <v>108</v>
+      </c>
+      <c r="L17" s="94"/>
+      <c r="M17" s="34"/>
+      <c r="O17" s="21"/>
+    </row>
+    <row r="18" spans="1:15" ht="30" customHeight="1">
+      <c r="A18" s="34"/>
+      <c r="B18" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="101"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="102" t="s">
-        <v>95</v>
-      </c>
-      <c r="J14" s="102"/>
-      <c r="K14" s="102" t="s">
-        <v>97</v>
-      </c>
-      <c r="L14" s="107" t="s">
-        <v>99</v>
-      </c>
-      <c r="M14" s="36"/>
-    </row>
-    <row r="15" spans="1:15" ht="30" customHeight="1">
-      <c r="A15" s="36"/>
-      <c r="B15" s="78" t="s">
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="96"/>
+      <c r="L18" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="34"/>
+      <c r="O18" s="21"/>
+    </row>
+    <row r="19" spans="1:15" ht="30" customHeight="1">
+      <c r="A19" s="34"/>
+      <c r="B19" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="85"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="100"/>
-      <c r="I15" s="85"/>
-      <c r="J15" s="85"/>
-      <c r="L15" s="91"/>
-      <c r="M15" s="36"/>
-      <c r="O15" s="23"/>
-    </row>
-    <row r="16" spans="1:15" ht="30" customHeight="1">
-      <c r="A16" s="36"/>
-      <c r="B16" s="95" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="101"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="102"/>
-      <c r="H16" s="103"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
-      <c r="K16" s="103"/>
-      <c r="L16" s="104" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="36"/>
-      <c r="O16" s="23"/>
-    </row>
-    <row r="17" spans="1:15" ht="30">
-      <c r="A17" s="36"/>
-      <c r="B17" s="78" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="85" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" s="85"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="88" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="85"/>
-      <c r="K17" s="100" t="s">
-        <v>115</v>
-      </c>
-      <c r="L17" s="91"/>
-      <c r="M17" s="36"/>
-      <c r="O17" s="23"/>
-    </row>
-    <row r="18" spans="1:15" ht="30" customHeight="1">
-      <c r="A18" s="36"/>
-      <c r="B18" s="95" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="101"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="102"/>
-      <c r="F18" s="102"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="103"/>
-      <c r="I18" s="102"/>
-      <c r="J18" s="102"/>
-      <c r="K18" s="103"/>
-      <c r="L18" s="104" t="s">
-        <v>10</v>
-      </c>
-      <c r="M18" s="36"/>
-      <c r="O18" s="23"/>
-    </row>
-    <row r="19" spans="1:15" ht="30" customHeight="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="92"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="93"/>
-      <c r="J19" s="93"/>
-      <c r="K19" s="108"/>
-      <c r="L19" s="94" t="s">
-        <v>10</v>
-      </c>
-      <c r="M19" s="36"/>
-      <c r="O19" s="23"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="98"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="34"/>
+      <c r="O19" s="21"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3286,7 +3034,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:N15"/>
   <sheetViews>
@@ -3308,15 +3056,15 @@
   <sheetData>
     <row r="7" spans="2:14">
       <c r="D7" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
       <c r="J7" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -3324,132 +3072,132 @@
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="2:14" ht="28" customHeight="1">
-      <c r="D8" s="44" t="s">
-        <v>105</v>
+      <c r="D8" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F8" s="2"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:14" ht="18">
-      <c r="B9" s="47" t="s">
-        <v>103</v>
+      <c r="B9" s="45" t="s">
+        <v>96</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="74" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="H9" s="47" t="s">
-        <v>103</v>
+      <c r="D9" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="H9" s="45" t="s">
+        <v>96</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="75"/>
+      <c r="J9" s="73"/>
     </row>
     <row r="10" spans="2:14" ht="18">
-      <c r="B10" s="47"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="H10" s="47"/>
+      <c r="D10" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="H10" s="45"/>
       <c r="I10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="75"/>
+      <c r="J10" s="73"/>
     </row>
     <row r="11" spans="2:14" ht="18">
-      <c r="B11" s="47"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="H11" s="47"/>
+      <c r="D11" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="H11" s="45"/>
       <c r="I11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="75"/>
+      <c r="J11" s="73"/>
     </row>
     <row r="12" spans="2:14" ht="18">
-      <c r="B12" s="47"/>
-      <c r="C12" s="45" t="s">
+      <c r="B12" s="45"/>
+      <c r="C12" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="75"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="45" t="s">
+      <c r="D12" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="73"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="75"/>
+      <c r="J12" s="73"/>
     </row>
     <row r="13" spans="2:14" ht="18">
-      <c r="B13" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="75"/>
-      <c r="H13" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="I13" s="45"/>
-      <c r="J13" s="75"/>
+      <c r="B13" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="73"/>
+      <c r="H13" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" s="43"/>
+      <c r="J13" s="73"/>
     </row>
     <row r="14" spans="2:14" ht="18">
-      <c r="B14" s="47"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="75"/>
-      <c r="H14" s="47"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="73"/>
+      <c r="H14" s="45"/>
       <c r="I14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="75"/>
+      <c r="J14" s="73"/>
     </row>
     <row r="15" spans="2:14" ht="18">
-      <c r="B15" s="47"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="75"/>
-      <c r="H15" s="47"/>
+        <v>86</v>
+      </c>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="73"/>
+      <c r="H15" s="45"/>
       <c r="I15" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J15" s="75"/>
+        <v>86</v>
+      </c>
+      <c r="J15" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3472,7 +3220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:E9"/>
   <sheetViews>
@@ -3488,33 +3236,33 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:5" ht="114" customHeight="1">
-      <c r="C5" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" s="78" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="76" t="s">
-        <v>108</v>
+      <c r="C5" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="74" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="80" customHeight="1">
-      <c r="C6" s="77"/>
-      <c r="D6" s="78" t="s">
-        <v>112</v>
-      </c>
-      <c r="E6" s="76" t="s">
-        <v>109</v>
+      <c r="C6" s="75"/>
+      <c r="D6" s="76" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="74" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="3:5">
       <c r="C8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="3:5">
       <c r="C9" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added important changes to related files.
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26800" yWindow="240" windowWidth="25600" windowHeight="15420" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-820" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId6"/>
     <sheet name="Sheet9" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="123">
   <si>
     <t>ACCESSIBILITY</t>
   </si>
@@ -466,6 +467,42 @@
   </si>
   <si>
     <t>e-service Quality dimensions (AUES)</t>
+  </si>
+  <si>
+    <t>2. Quality concept</t>
+  </si>
+  <si>
+    <t>1. Services concept</t>
+  </si>
+  <si>
+    <t>3. Service quality</t>
+  </si>
+  <si>
+    <t>4. Definitions of e-service</t>
+  </si>
+  <si>
+    <t>5. ISO/IEC 25010:2011</t>
+  </si>
+  <si>
+    <t>6. e-service quality</t>
+  </si>
+  <si>
+    <t>7, IT-Services</t>
+  </si>
+  <si>
+    <t>8. E-Commerce</t>
+  </si>
+  <si>
+    <t>9. E-Government</t>
+  </si>
+  <si>
+    <t>10. E-Infrastructure</t>
+  </si>
+  <si>
+    <t>11. E-Services Providers</t>
+  </si>
+  <si>
+    <t>12.Online and traditional business environment</t>
   </si>
 </sst>
 </file>
@@ -790,7 +827,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="201">
+  <cellStyleXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -992,8 +1029,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1058,12 +1113,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1073,14 +1122,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1121,6 +1164,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1292,8 +1338,32 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="201">
+  <cellStyles count="219">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1394,6 +1464,15 @@
     <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1494,6 +1573,15 @@
     <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1823,140 +1911,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="8" width="12.83203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="21" customHeight="1">
-      <c r="B2" s="22"/>
+    <row r="1" spans="1:9">
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" customHeight="1">
+      <c r="A2" s="30"/>
+      <c r="B2" s="22" t="s">
+        <v>12</v>
+      </c>
       <c r="C2" s="23"/>
-      <c r="D2" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26"/>
-    </row>
-    <row r="3" spans="2:9" s="21" customFormat="1" ht="20" customHeight="1">
-      <c r="B3" s="27"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="28" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="30"/>
+    </row>
+    <row r="3" spans="1:9" s="21" customFormat="1" ht="20" customHeight="1">
+      <c r="A3" s="32"/>
+      <c r="B3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="C3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="D3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="E3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="F3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="G3" s="25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" s="11" customFormat="1" ht="21" customHeight="1">
-      <c r="B4" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="30" t="s">
+      <c r="H3" s="105"/>
+      <c r="I3" s="32"/>
+    </row>
+    <row r="4" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1">
+      <c r="A4" s="106"/>
+      <c r="B4" s="100" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="2:9" s="11" customFormat="1" ht="21" customHeight="1">
-      <c r="B5" s="29"/>
-      <c r="C5" s="31" t="s">
+      <c r="I4" s="106"/>
+    </row>
+    <row r="5" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1">
+      <c r="A5" s="106"/>
+      <c r="B5" s="101" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="2:9" s="11" customFormat="1" ht="21" customHeight="1">
-      <c r="B6" s="29"/>
-      <c r="C6" s="32" t="s">
+      <c r="I5" s="106"/>
+    </row>
+    <row r="6" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1">
+      <c r="A6" s="106"/>
+      <c r="B6" s="102" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="17"/>
-    </row>
-    <row r="7" spans="2:9" s="11" customFormat="1" ht="21" customHeight="1">
-      <c r="B7" s="29"/>
-      <c r="C7" s="33" t="s">
+      <c r="I6" s="106"/>
+    </row>
+    <row r="7" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1">
+      <c r="A7" s="106"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="I7" s="106"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B2:C3"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1983,90 +2095,90 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" thickBot="1">
-      <c r="A3" s="34"/>
-      <c r="B3" s="37" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="30"/>
     </row>
     <row r="4" spans="1:4" ht="26" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="34"/>
-      <c r="B4" s="39" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A5" s="34"/>
-      <c r="B5" s="39" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="30"/>
     </row>
     <row r="6" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A6" s="34"/>
-      <c r="B6" s="39" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="30"/>
     </row>
     <row r="7" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A7" s="34"/>
-      <c r="B7" s="39" t="s">
+      <c r="A7" s="30"/>
+      <c r="B7" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="30"/>
     </row>
     <row r="8" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A8" s="34"/>
-      <c r="B8" s="39" t="s">
+      <c r="A8" s="30"/>
+      <c r="B8" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="30"/>
     </row>
     <row r="9" spans="1:4" ht="26" customHeight="1" thickBot="1">
-      <c r="A9" s="34"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="40" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="30"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2101,81 +2213,81 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="36"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="2:8" ht="24" customHeight="1">
-      <c r="B3" s="34"/>
-      <c r="C3" s="77" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="74" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="34"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="2:8" ht="27" customHeight="1">
-      <c r="B4" s="36"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="83" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="76" t="s">
+      <c r="F4" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="76" t="s">
+      <c r="G4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="34"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="B5" s="35"/>
-      <c r="C5" s="85" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="87" t="s">
+      <c r="E5" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="88" t="s">
+      <c r="F5" s="84" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="35"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="2:8" ht="20" customHeight="1">
-      <c r="B6" s="36"/>
-      <c r="C6" s="76" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="89" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="90" t="s">
+      <c r="D6" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="90"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="34"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="2:8" ht="20" customHeight="1">
-      <c r="B7" s="36"/>
-      <c r="C7" s="82" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="79" t="s">
         <v>55</v>
       </c>
       <c r="D7" s="4"/>
@@ -2186,26 +2298,26 @@
         <v>56</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="34"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="2:8" ht="20" customHeight="1">
-      <c r="B8" s="34"/>
-      <c r="C8" s="84" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="89"/>
-      <c r="E8" s="90" t="s">
+      <c r="D8" s="86"/>
+      <c r="E8" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="90" t="s">
+      <c r="F8" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="91"/>
-      <c r="H8" s="34"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="2:8" ht="20" customHeight="1">
-      <c r="B9" s="34"/>
-      <c r="C9" s="82" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="79" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -2216,28 +2328,28 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="34"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:8" ht="20" customHeight="1">
-      <c r="B10" s="34"/>
-      <c r="C10" s="76" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="89"/>
-      <c r="E10" s="90" t="s">
+      <c r="D10" s="86"/>
+      <c r="E10" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="90" t="s">
+      <c r="F10" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="91" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="34"/>
+      <c r="G10" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:8" ht="20" customHeight="1">
-      <c r="B11" s="34"/>
-      <c r="C11" s="82" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="79" t="s">
         <v>46</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -2250,26 +2362,26 @@
       <c r="G11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="34"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:8" ht="20" customHeight="1">
-      <c r="B12" s="34"/>
-      <c r="C12" s="84" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="89"/>
-      <c r="E12" s="90" t="s">
+      <c r="D12" s="86"/>
+      <c r="E12" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="90"/>
+      <c r="F12" s="87"/>
       <c r="G12" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="34"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" ht="20" customHeight="1">
-      <c r="B13" s="34"/>
-      <c r="C13" s="82" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="79" t="s">
         <v>53</v>
       </c>
       <c r="D13" s="8"/>
@@ -2278,21 +2390,21 @@
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="34"/>
+      <c r="H13" s="30"/>
     </row>
     <row r="14" spans="2:8" ht="23" customHeight="1">
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35" t="s">
+      <c r="B14" s="30"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="34"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="30"/>
     </row>
     <row r="15" spans="2:8">
-      <c r="C15" s="44"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -2335,14 +2447,14 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="3:7">
-      <c r="C22" s="46"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="3:7">
-      <c r="C23" s="46"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2381,155 +2493,155 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="34"/>
-      <c r="B3" s="51" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="34"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" ht="25" customHeight="1">
-      <c r="A4" s="34"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="53" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="34"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="47" t="s">
+      <c r="A5" s="31"/>
+      <c r="B5" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="66"/>
-      <c r="G5" s="35"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="63"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A6" s="35"/>
-      <c r="B6" s="54" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="56" t="s">
+      <c r="C6" s="52"/>
+      <c r="D6" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="57" t="s">
+      <c r="F6" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="35"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A7" s="35"/>
-      <c r="B7" s="67" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="35"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="66"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="31"/>
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="35"/>
-      <c r="B8" s="54" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="56" t="s">
+      <c r="C8" s="52"/>
+      <c r="D8" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="58" t="s">
+      <c r="F8" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="35"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A9" s="35"/>
-      <c r="B9" s="70" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49" t="s">
+      <c r="C9" s="45"/>
+      <c r="D9" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="35"/>
+      <c r="F9" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="A10" s="35"/>
-      <c r="B10" s="54" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60" t="s">
+      <c r="C10" s="56"/>
+      <c r="D10" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="61" t="s">
+      <c r="E10" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="35"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2549,7 +2661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -2572,452 +2684,452 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:15" ht="22" customHeight="1">
-      <c r="A2" s="34"/>
-      <c r="B2" s="81" t="s">
+      <c r="A2" s="30"/>
+      <c r="B2" s="78" t="s">
         <v>109</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="34"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="30"/>
       <c r="N2" s="21"/>
     </row>
     <row r="3" spans="1:15" ht="39" customHeight="1">
-      <c r="A3" s="34"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="80" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="74" t="s">
+      <c r="E3" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="74" t="s">
+      <c r="H3" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="79" t="s">
+      <c r="I3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="74" t="s">
+      <c r="J3" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="78" t="s">
+      <c r="K3" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="74" t="s">
+      <c r="L3" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="M3" s="36"/>
+      <c r="M3" s="32"/>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1">
-      <c r="A4" s="34"/>
-      <c r="B4" s="82" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92" t="s">
+      <c r="C4" s="89"/>
+      <c r="D4" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="93" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92" t="s">
+      <c r="E4" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92" t="s">
+      <c r="H4" s="89"/>
+      <c r="I4" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="93" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="34"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="30"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1">
-      <c r="A5" s="34"/>
-      <c r="B5" s="76" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="94"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="95" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="34"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="30"/>
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1">
-      <c r="A6" s="34"/>
-      <c r="B6" s="82" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="92" t="s">
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92" t="s">
+      <c r="H6" s="89"/>
+      <c r="I6" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="93" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="34"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="30"/>
     </row>
     <row r="7" spans="1:15" ht="30">
-      <c r="A7" s="34"/>
-      <c r="B7" s="76" t="s">
+      <c r="A7" s="30"/>
+      <c r="B7" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="94" t="s">
+      <c r="C7" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="94"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="99"/>
-      <c r="M7" s="34"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="96"/>
+      <c r="M7" s="30"/>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1">
-      <c r="A8" s="34"/>
-      <c r="B8" s="82" t="s">
+      <c r="A8" s="30"/>
+      <c r="B8" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92" t="s">
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="96"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="93" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="34"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="30"/>
     </row>
     <row r="9" spans="1:15" ht="30">
-      <c r="A9" s="34"/>
-      <c r="B9" s="76" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="94" t="s">
+      <c r="E9" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="94" t="s">
+      <c r="F9" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94" t="s">
+      <c r="G9" s="91"/>
+      <c r="H9" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94" t="s">
+      <c r="I9" s="91"/>
+      <c r="J9" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="K9" s="94" t="s">
+      <c r="K9" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="L9" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="34"/>
+      <c r="L9" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="30"/>
     </row>
     <row r="10" spans="1:15" ht="30" customHeight="1">
-      <c r="A10" s="34"/>
-      <c r="B10" s="82" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92" t="s">
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92" t="s">
+      <c r="I10" s="89"/>
+      <c r="J10" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="K10" s="92"/>
-      <c r="L10" s="93" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="34"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="30"/>
     </row>
     <row r="11" spans="1:15" ht="30">
-      <c r="A11" s="34"/>
-      <c r="B11" s="76" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="94" t="s">
+      <c r="C11" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="94"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="34"/>
+      <c r="D11" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="96"/>
+      <c r="M11" s="30"/>
     </row>
     <row r="12" spans="1:15" ht="30" customHeight="1">
-      <c r="A12" s="34"/>
-      <c r="B12" s="82" t="s">
+      <c r="A12" s="30"/>
+      <c r="B12" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="93" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="100"/>
-      <c r="M12" s="34"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="97"/>
+      <c r="M12" s="30"/>
     </row>
     <row r="13" spans="1:15" ht="30">
-      <c r="A13" s="34"/>
-      <c r="B13" s="76" t="s">
+      <c r="A13" s="30"/>
+      <c r="B13" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="94" t="s">
+      <c r="C13" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="94" t="s">
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="94" t="s">
+      <c r="G13" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="M13" s="34"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="30"/>
     </row>
     <row r="14" spans="1:15" ht="37" customHeight="1">
-      <c r="A14" s="34"/>
-      <c r="B14" s="82" t="s">
+      <c r="A14" s="30"/>
+      <c r="B14" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92" t="s">
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92" t="s">
+      <c r="J14" s="89"/>
+      <c r="K14" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="L14" s="92" t="s">
+      <c r="L14" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="M14" s="34"/>
+      <c r="M14" s="30"/>
     </row>
     <row r="15" spans="1:15" ht="30" customHeight="1">
-      <c r="A15" s="34"/>
-      <c r="B15" s="76" t="s">
+      <c r="A15" s="30"/>
+      <c r="B15" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="94"/>
-      <c r="G15" s="94"/>
-      <c r="H15" s="98"/>
-      <c r="I15" s="94"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="101"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="34"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="91"/>
+      <c r="M15" s="30"/>
       <c r="O15" s="21"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1">
-      <c r="A16" s="34"/>
-      <c r="B16" s="82" t="s">
+      <c r="A16" s="30"/>
+      <c r="B16" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="96"/>
-      <c r="L16" s="93" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="34"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="89"/>
+      <c r="J16" s="89"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="30"/>
       <c r="O16" s="21"/>
     </row>
     <row r="17" spans="1:15" ht="30">
-      <c r="A17" s="34"/>
-      <c r="B17" s="76" t="s">
+      <c r="A17" s="30"/>
+      <c r="B17" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94" t="s">
+      <c r="C17" s="91"/>
+      <c r="D17" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="98"/>
-      <c r="I17" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="94"/>
-      <c r="K17" s="98" t="s">
+      <c r="E17" s="91"/>
+      <c r="F17" s="91"/>
+      <c r="G17" s="91"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="91"/>
+      <c r="K17" s="95" t="s">
         <v>108</v>
       </c>
-      <c r="L17" s="94"/>
-      <c r="M17" s="34"/>
+      <c r="L17" s="91"/>
+      <c r="M17" s="30"/>
       <c r="O17" s="21"/>
     </row>
     <row r="18" spans="1:15" ht="30" customHeight="1">
-      <c r="A18" s="34"/>
-      <c r="B18" s="82" t="s">
+      <c r="A18" s="30"/>
+      <c r="B18" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="96"/>
-      <c r="L18" s="93" t="s">
-        <v>10</v>
-      </c>
-      <c r="M18" s="34"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="30"/>
       <c r="O18" s="21"/>
     </row>
     <row r="19" spans="1:15" ht="30" customHeight="1">
-      <c r="A19" s="34"/>
-      <c r="B19" s="76" t="s">
+      <c r="A19" s="30"/>
+      <c r="B19" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="94"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="94"/>
-      <c r="G19" s="94"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="94"/>
-      <c r="J19" s="94"/>
-      <c r="K19" s="98"/>
-      <c r="L19" s="99" t="s">
-        <v>10</v>
-      </c>
-      <c r="M19" s="34"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="91"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="91"/>
+      <c r="J19" s="91"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="96" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="30"/>
       <c r="O19" s="21"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3060,9 +3172,9 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
       <c r="J7" s="3" t="s">
         <v>100</v>
       </c>
@@ -3072,7 +3184,7 @@
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="2:14" ht="28" customHeight="1">
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="38" t="s">
         <v>98</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -3082,122 +3194,122 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:14" ht="18">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="42" t="s">
         <v>96</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="H9" s="45" t="s">
+      <c r="D9" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="H9" s="42" t="s">
         <v>96</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="73"/>
+      <c r="J9" s="70"/>
     </row>
     <row r="10" spans="2:14" ht="18">
-      <c r="B10" s="45"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="H10" s="45"/>
+      <c r="D10" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="H10" s="42"/>
       <c r="I10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="73"/>
+      <c r="J10" s="70"/>
     </row>
     <row r="11" spans="2:14" ht="18">
-      <c r="B11" s="45"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="H11" s="45"/>
+      <c r="D11" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="H11" s="42"/>
       <c r="I11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="73"/>
+      <c r="J11" s="70"/>
     </row>
     <row r="12" spans="2:14" ht="18">
-      <c r="B12" s="45"/>
-      <c r="C12" s="43" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="73"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="43" t="s">
+      <c r="D12" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="70"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="73"/>
+      <c r="J12" s="70"/>
     </row>
     <row r="13" spans="2:14" ht="18">
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="73"/>
-      <c r="H13" s="45" t="s">
+      <c r="C13" s="39"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="70"/>
+      <c r="H13" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="I13" s="43"/>
-      <c r="J13" s="73"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="70"/>
     </row>
     <row r="14" spans="2:14" ht="18">
-      <c r="B14" s="45"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="73"/>
-      <c r="H14" s="45"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="70"/>
+      <c r="H14" s="42"/>
       <c r="I14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="73"/>
+      <c r="J14" s="70"/>
     </row>
     <row r="15" spans="2:14" ht="18">
-      <c r="B15" s="45"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="73"/>
-      <c r="H15" s="45"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="70"/>
+      <c r="H15" s="42"/>
       <c r="I15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J15" s="73"/>
+      <c r="J15" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3236,22 +3348,22 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:5" ht="114" customHeight="1">
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="E5" s="71" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="80" customHeight="1">
-      <c r="C6" s="75"/>
-      <c r="D6" s="76" t="s">
+      <c r="C6" s="72"/>
+      <c r="D6" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="74" t="s">
+      <c r="E6" s="71" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3277,4 +3389,77 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="36" customHeight="1">
+      <c r="B2" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="36" customHeight="1">
+      <c r="B3" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="36" customHeight="1">
+      <c r="B4" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="36" customHeight="1">
+      <c r="B5" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="36" customHeight="1">
+      <c r="B6" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="36" customHeight="1">
+      <c r="B7" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="99" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed customer support dimensional component.
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-820" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="500" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="-820" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="500" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
     <sheet name="Sheet10" sheetId="10" r:id="rId8"/>
     <sheet name="Sheet11" sheetId="11" r:id="rId9"/>
     <sheet name="Provider view" sheetId="12" r:id="rId10"/>
-    <sheet name="User view" sheetId="15" r:id="rId11"/>
-    <sheet name="Questionaire" sheetId="17" r:id="rId12"/>
+    <sheet name="Questionaire" sheetId="17" r:id="rId11"/>
+    <sheet name="User view" sheetId="15" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="188">
   <si>
     <t>ACCESSIBILITY</t>
   </si>
@@ -533,9 +533,6 @@
     <t>e-service product quality</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>Sum</t>
   </si>
   <si>
@@ -572,9 +569,6 @@
     <t>The graphic interface was clear and comprehensive?</t>
   </si>
   <si>
-    <t>The e-service was fully available without any interruption problems</t>
-  </si>
-  <si>
     <t>Did you face any response problems?</t>
   </si>
   <si>
@@ -684,6 +678,30 @@
   </si>
   <si>
     <t>Customer service</t>
+  </si>
+  <si>
+    <t>availability</t>
+  </si>
+  <si>
+    <t>Did you authenticate yourself for using the e-service?</t>
+  </si>
+  <si>
+    <t>Were you informed your information is not shared with third parties without your authorization?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Was the information related to you or your transaction altered of modified during using the service?</t>
+  </si>
+  <si>
+    <t>Did you noticed any kind of informaton not related to you or your transaction during using the service?</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Do you trust on the service for accomplishing your goals?</t>
   </si>
 </sst>
 </file>
@@ -761,7 +779,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -783,6 +801,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1017,7 +1041,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="293">
+  <cellStyleXfs count="301">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1311,8 +1335,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1451,6 +1483,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1717,29 +1750,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="293">
+  <cellStyles count="301">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1886,6 +1931,10 @@
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2032,6 +2081,10 @@
     <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2398,7 +2451,7 @@
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
       <c r="H2" s="27"/>
-      <c r="I2" s="108" t="s">
+      <c r="I2" s="109" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="33"/>
@@ -2423,12 +2476,12 @@
       <c r="H3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="109"/>
+      <c r="I3" s="110"/>
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="2:10" s="14" customFormat="1" ht="21" customHeight="1">
-      <c r="B4" s="110"/>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="111"/>
+      <c r="C4" s="105" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -2445,11 +2498,11 @@
       <c r="I4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="110"/>
+      <c r="J4" s="111"/>
     </row>
     <row r="5" spans="2:10" s="14" customFormat="1" ht="21" customHeight="1">
-      <c r="B5" s="110"/>
-      <c r="C5" s="105" t="s">
+      <c r="B5" s="111"/>
+      <c r="C5" s="106" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="17"/>
@@ -2462,11 +2515,11 @@
       <c r="I5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="110"/>
+      <c r="J5" s="111"/>
     </row>
     <row r="6" spans="2:10" s="14" customFormat="1" ht="21" customHeight="1">
-      <c r="B6" s="110"/>
-      <c r="C6" s="106" t="s">
+      <c r="B6" s="111"/>
+      <c r="C6" s="107" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="19" t="s">
@@ -2483,11 +2536,11 @@
       <c r="I6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="110"/>
+      <c r="J6" s="111"/>
     </row>
     <row r="7" spans="2:10" s="14" customFormat="1" ht="21" customHeight="1">
-      <c r="B7" s="110"/>
-      <c r="C7" s="107"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="108"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21" t="s">
         <v>10</v>
@@ -2502,7 +2555,7 @@
       <c r="I7" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="110"/>
+      <c r="J7" s="111"/>
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="33"/>
@@ -2524,7 +2577,7 @@
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
       <c r="H12" s="27"/>
-      <c r="I12" s="111" t="s">
+      <c r="I12" s="112" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2547,10 +2600,10 @@
       <c r="H13" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="112"/>
+      <c r="I13" s="113"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="C14" s="104">
+      <c r="C14" s="105">
         <v>1</v>
       </c>
       <c r="D14" s="15">
@@ -2572,7 +2625,7 @@
       </c>
     </row>
     <row r="15" spans="2:10">
-      <c r="C15" s="105">
+      <c r="C15" s="106">
         <v>1</v>
       </c>
       <c r="D15" s="17"/>
@@ -2590,7 +2643,7 @@
       </c>
     </row>
     <row r="16" spans="2:10">
-      <c r="C16" s="106">
+      <c r="C16" s="107">
         <v>1</v>
       </c>
       <c r="D16" s="19">
@@ -2612,7 +2665,7 @@
       </c>
     </row>
     <row r="17" spans="3:10">
-      <c r="C17" s="107"/>
+      <c r="C17" s="108"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21">
         <v>1</v>
@@ -2757,57 +2810,57 @@
     <col min="14" max="14" width="3.83203125" customWidth="1"/>
     <col min="15" max="15" width="16.33203125" customWidth="1"/>
     <col min="16" max="16" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5" style="113" customWidth="1"/>
+    <col min="17" max="17" width="14.5" style="114" customWidth="1"/>
     <col min="18" max="18" width="3.83203125" customWidth="1"/>
     <col min="19" max="19" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:22">
-      <c r="D2" s="131" t="s">
+      <c r="D2" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="132" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="132" t="s">
+      <c r="E2" s="133" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="133" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="135" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="134" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="3" spans="2:22">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="83" t="s">
         <v>129</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="77">
+      <c r="D3" s="78">
         <f>$K$12</f>
         <v>4.5</v>
       </c>
-      <c r="E3" s="77">
+      <c r="E3" s="78">
         <f>$K$16</f>
         <v>2.5</v>
       </c>
-      <c r="F3" s="77">
+      <c r="F3" s="78">
         <f>$K$19</f>
         <v>2</v>
       </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77">
+      <c r="G3" s="78"/>
+      <c r="H3" s="78">
         <f>SUM(D3:G3)</f>
         <v>9</v>
       </c>
-      <c r="I3" s="137">
+      <c r="I3" s="138">
         <f>SUM(H3:H5)</f>
         <v>17.166666666666668</v>
       </c>
@@ -2817,47 +2870,47 @@
       </c>
     </row>
     <row r="4" spans="2:22">
-      <c r="B4" s="82"/>
+      <c r="B4" s="83"/>
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="77">
+      <c r="D4" s="78">
         <f>$K$12</f>
         <v>4.5</v>
       </c>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77">
+      <c r="E4" s="78"/>
+      <c r="F4" s="78">
         <f>$K$19</f>
         <v>2</v>
       </c>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77">
+      <c r="G4" s="78"/>
+      <c r="H4" s="78">
         <f>SUM(D4:G4)</f>
         <v>6.5</v>
       </c>
-      <c r="I4" s="137"/>
+      <c r="I4" s="138"/>
       <c r="J4" s="2"/>
       <c r="V4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="5" spans="2:22">
-      <c r="B5" s="82"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="135">
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="136">
         <f>$K$24</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="H5" s="136">
+      <c r="H5" s="137">
         <f>SUM(D5:G5)</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="I5" s="137"/>
+      <c r="I5" s="138"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="2:22">
@@ -2867,75 +2920,75 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:22">
-      <c r="B7" s="133" t="s">
+      <c r="B7" s="134" t="s">
         <v>130</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="77">
+      <c r="D7" s="78">
         <f>$K$12</f>
         <v>4.5</v>
       </c>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77">
+      <c r="E7" s="78"/>
+      <c r="F7" s="78">
         <f>$K$19</f>
         <v>2</v>
       </c>
-      <c r="G7" s="135">
+      <c r="G7" s="136">
         <f>$K$24</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="H7" s="136">
+      <c r="H7" s="137">
         <f>SUM(D7:G7)</f>
         <v>8.1666666666666661</v>
       </c>
-      <c r="I7" s="137">
+      <c r="I7" s="138">
         <f>SUM(H7:H9)</f>
         <v>18.833333333333332</v>
       </c>
     </row>
     <row r="8" spans="2:22">
-      <c r="B8" s="133"/>
+      <c r="B8" s="134"/>
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="77">
+      <c r="D8" s="78">
         <f>$K$12</f>
         <v>4.5</v>
       </c>
-      <c r="E8" s="77">
+      <c r="E8" s="78">
         <f>$K$16</f>
         <v>2.5</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="78">
         <f>$K$19</f>
         <v>2</v>
       </c>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77">
+      <c r="G8" s="78"/>
+      <c r="H8" s="78">
         <f t="shared" ref="H8:H9" si="0">SUM(D8:G8)</f>
         <v>9</v>
       </c>
-      <c r="I8" s="137"/>
+      <c r="I8" s="138"/>
     </row>
     <row r="9" spans="2:22">
-      <c r="B9" s="133"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="135">
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="136">
         <f>$K$24</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="H9" s="136">
+      <c r="H9" s="137">
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="I9" s="137"/>
+      <c r="I9" s="138"/>
     </row>
     <row r="10" spans="2:22" ht="4" customHeight="1"/>
     <row r="11" spans="2:22">
@@ -2963,46 +3016,46 @@
       </c>
     </row>
     <row r="13" spans="2:22" ht="20" customHeight="1">
-      <c r="K13" s="122" t="s">
+      <c r="K13" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="L13" s="119">
+      <c r="L13" s="120">
         <f>N13+N14+N15+P14+P15</f>
         <v>18</v>
       </c>
-      <c r="M13" s="77" t="s">
+      <c r="M13" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="N13" s="124">
+      <c r="N13" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:22" ht="36" customHeight="1">
-      <c r="K14" s="122"/>
-      <c r="L14" s="120"/>
-      <c r="M14" s="78" t="s">
+      <c r="K14" s="123"/>
+      <c r="L14" s="121"/>
+      <c r="M14" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="N14" s="124">
-        <v>1</v>
-      </c>
-      <c r="O14" s="78" t="s">
+      <c r="N14" s="125">
+        <v>1</v>
+      </c>
+      <c r="O14" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="P14" s="124">
+      <c r="P14" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:22" ht="25" customHeight="1">
-      <c r="K15" s="122"/>
-      <c r="L15" s="121"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="123">
+      <c r="K15" s="123"/>
+      <c r="L15" s="122"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="124">
         <f>P14+P15</f>
         <v>8</v>
       </c>
-      <c r="O15" s="78"/>
-      <c r="P15" s="123">
+      <c r="O15" s="79"/>
+      <c r="P15" s="124">
         <f>N17+N18+N20+N21+N22</f>
         <v>7</v>
       </c>
@@ -3014,44 +3067,44 @@
       </c>
     </row>
     <row r="17" spans="11:20">
-      <c r="K17" s="119" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" s="119">
+      <c r="K17" s="120" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="120">
         <f>N17+N18+P17+P18+R18</f>
         <v>5</v>
       </c>
-      <c r="M17" s="78" t="s">
+      <c r="M17" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="N17" s="124">
-        <v>1</v>
-      </c>
-      <c r="O17" s="78" t="s">
+      <c r="N17" s="125">
+        <v>1</v>
+      </c>
+      <c r="O17" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="P17" s="127">
+      <c r="P17" s="128">
         <v>1</v>
       </c>
       <c r="Q17"/>
     </row>
     <row r="18" spans="11:20" ht="34" customHeight="1">
-      <c r="K18" s="121"/>
-      <c r="L18" s="121"/>
-      <c r="M18" s="78"/>
-      <c r="N18" s="123">
+      <c r="K18" s="122"/>
+      <c r="L18" s="122"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="124">
         <f>P17:P18</f>
         <v>1</v>
       </c>
-      <c r="O18" s="78"/>
-      <c r="P18" s="123">
+      <c r="O18" s="79"/>
+      <c r="P18" s="124">
         <f>R18</f>
         <v>1</v>
       </c>
-      <c r="Q18" s="81" t="s">
+      <c r="Q18" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="R18" s="124">
+      <c r="R18" s="125">
         <v>1</v>
       </c>
     </row>
@@ -3062,146 +3115,146 @@
       </c>
     </row>
     <row r="20" spans="11:20" ht="20" customHeight="1">
-      <c r="K20" s="119" t="s">
+      <c r="K20" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="119">
+      <c r="L20" s="120">
         <f>N20+N21+N22+P21+P22+P23</f>
         <v>8</v>
       </c>
       <c r="M20" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="N20" s="125">
+      <c r="N20" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="11:20" ht="20" customHeight="1">
-      <c r="K21" s="120"/>
-      <c r="L21" s="120"/>
-      <c r="M21" s="116" t="s">
+      <c r="K21" s="121"/>
+      <c r="L21" s="121"/>
+      <c r="M21" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="N21" s="125">
-        <v>1</v>
-      </c>
-      <c r="O21" s="75" t="s">
+      <c r="N21" s="126">
+        <v>1</v>
+      </c>
+      <c r="O21" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="P21" s="125">
+      <c r="P21" s="126">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="11:20" ht="20" customHeight="1">
-      <c r="K22" s="120"/>
-      <c r="L22" s="120"/>
-      <c r="M22" s="117"/>
-      <c r="N22" s="108">
+      <c r="K22" s="121"/>
+      <c r="L22" s="121"/>
+      <c r="M22" s="118"/>
+      <c r="N22" s="109">
         <f>P21+P22+P23</f>
         <v>3</v>
       </c>
-      <c r="O22" s="138" t="s">
+      <c r="O22" s="139" t="s">
         <v>128</v>
       </c>
-      <c r="P22" s="126">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="138" t="s">
+      <c r="P22" s="127">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="R22" s="138">
+      <c r="R22" s="139">
         <f>T22+T23</f>
         <v>2</v>
       </c>
-      <c r="S22" s="115" t="s">
+      <c r="S22" s="116" t="s">
         <v>126</v>
       </c>
-      <c r="T22" s="125">
+      <c r="T22" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="11:20" ht="20" customHeight="1">
-      <c r="K23" s="121"/>
-      <c r="L23" s="121"/>
-      <c r="M23" s="118"/>
-      <c r="N23" s="109"/>
-      <c r="O23" s="139"/>
-      <c r="P23" s="123">
+      <c r="K23" s="122"/>
+      <c r="L23" s="122"/>
+      <c r="M23" s="119"/>
+      <c r="N23" s="110"/>
+      <c r="O23" s="140"/>
+      <c r="P23" s="124">
         <f>R22</f>
         <v>2</v>
       </c>
-      <c r="Q23" s="139"/>
-      <c r="R23" s="139"/>
-      <c r="S23" s="115" t="s">
+      <c r="Q23" s="140"/>
+      <c r="R23" s="140"/>
+      <c r="S23" s="116" t="s">
         <v>127</v>
       </c>
-      <c r="T23" s="125">
+      <c r="T23" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="11:20">
-      <c r="K24" s="130">
+      <c r="K24" s="131">
         <f>L25/3</f>
         <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="25" spans="11:20" ht="20" customHeight="1">
-      <c r="K25" s="119" t="s">
+      <c r="K25" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="L25" s="119">
+      <c r="L25" s="120">
         <f>N26+N25</f>
         <v>5</v>
       </c>
-      <c r="M25" s="116" t="s">
+      <c r="M25" s="117" t="s">
         <v>37</v>
       </c>
-      <c r="N25" s="124">
-        <v>1</v>
-      </c>
-      <c r="O25" s="114" t="s">
+      <c r="N25" s="125">
+        <v>1</v>
+      </c>
+      <c r="O25" s="115" t="s">
         <v>38</v>
       </c>
-      <c r="P25" s="124">
+      <c r="P25" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="11:20" ht="20" customHeight="1">
-      <c r="K26" s="120"/>
-      <c r="L26" s="120"/>
-      <c r="M26" s="117"/>
-      <c r="N26" s="119">
+      <c r="K26" s="121"/>
+      <c r="L26" s="121"/>
+      <c r="M26" s="118"/>
+      <c r="N26" s="120">
         <f>P25+P26+P27+P28</f>
         <v>4</v>
       </c>
-      <c r="O26" s="114" t="s">
+      <c r="O26" s="115" t="s">
         <v>39</v>
       </c>
-      <c r="P26" s="124">
+      <c r="P26" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="11:20" ht="20" customHeight="1">
-      <c r="K27" s="120"/>
-      <c r="L27" s="120"/>
-      <c r="M27" s="117"/>
-      <c r="N27" s="120"/>
-      <c r="O27" s="114" t="s">
+      <c r="K27" s="121"/>
+      <c r="L27" s="121"/>
+      <c r="M27" s="118"/>
+      <c r="N27" s="121"/>
+      <c r="O27" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="P27" s="124">
+      <c r="P27" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="11:20" ht="20" customHeight="1">
-      <c r="K28" s="121"/>
-      <c r="L28" s="121"/>
-      <c r="M28" s="118"/>
-      <c r="N28" s="121"/>
-      <c r="O28" s="114" t="s">
+      <c r="K28" s="122"/>
+      <c r="L28" s="122"/>
+      <c r="M28" s="119"/>
+      <c r="N28" s="122"/>
+      <c r="O28" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="P28" s="124">
+      <c r="P28" s="125">
         <v>1</v>
       </c>
     </row>
@@ -3243,10 +3296,488 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:H63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="4" style="1" customWidth="1"/>
+    <col min="4" max="4" width="64.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="65.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:8">
+      <c r="C3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="C5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="D9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="D10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="D12" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" t="s">
+        <v>170</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14">
+        <v>0.5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="D15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="D17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" t="s">
+        <v>170</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="D18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" t="s">
+        <v>168</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="D22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22">
+        <v>0.5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="D23" t="s">
+        <v>167</v>
+      </c>
+      <c r="E23" t="s">
+        <v>170</v>
+      </c>
+      <c r="F23">
+        <v>0.5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="D25" t="s">
+        <v>178</v>
+      </c>
+      <c r="E25" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="D27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E27" t="s">
+        <v>170</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="D29" t="s">
+        <v>182</v>
+      </c>
+      <c r="E29" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="D31" t="s">
+        <v>184</v>
+      </c>
+      <c r="E31" t="s">
+        <v>183</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="D33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E33" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="D35" t="s">
+        <v>166</v>
+      </c>
+      <c r="E35" t="s">
+        <v>170</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="D37" t="s">
+        <v>187</v>
+      </c>
+      <c r="E37" t="s">
+        <v>170</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="D41" s="48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="C42" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="C43" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="D47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="D51" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" t="s">
+        <v>87</v>
+      </c>
+      <c r="D52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="D54" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="D56" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="D57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="D58" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="D60" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="D61" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="D62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="D63" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C42:H42"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="M9" sqref="M9:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3267,7 +3798,7 @@
     <col min="14" max="14" width="3.83203125" customWidth="1"/>
     <col min="15" max="15" width="16.33203125" customWidth="1"/>
     <col min="16" max="16" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5" style="113" customWidth="1"/>
+    <col min="17" max="17" width="14.5" style="114" customWidth="1"/>
     <col min="18" max="18" width="3.83203125" customWidth="1"/>
     <col min="19" max="19" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.83203125" customWidth="1"/>
@@ -3288,47 +3819,47 @@
       </c>
     </row>
     <row r="2" spans="2:22">
-      <c r="D2" s="131" t="s">
+      <c r="D2" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="132" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="132" t="s">
+      <c r="E2" s="133" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="133" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="135" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="134" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="3" spans="2:22">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="83" t="s">
         <v>129</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="77">
-        <v>1</v>
-      </c>
-      <c r="E3" s="77">
-        <v>1</v>
-      </c>
-      <c r="F3" s="77">
-        <v>1</v>
-      </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77">
+      <c r="D3" s="78">
+        <v>1</v>
+      </c>
+      <c r="E3" s="78">
+        <v>1</v>
+      </c>
+      <c r="F3" s="78">
+        <v>1</v>
+      </c>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78">
         <f>SUM(D3:G3)</f>
         <v>3</v>
       </c>
-      <c r="I3" s="137">
+      <c r="I3" s="138">
         <f>SUM(H3:H5)</f>
         <v>6</v>
       </c>
@@ -3338,44 +3869,44 @@
       </c>
     </row>
     <row r="4" spans="2:22">
-      <c r="B4" s="82"/>
+      <c r="B4" s="83"/>
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="77">
-        <v>1</v>
-      </c>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77">
-        <v>1</v>
-      </c>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77">
+      <c r="D4" s="78">
+        <v>1</v>
+      </c>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78">
+        <v>1</v>
+      </c>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78">
         <f>SUM(D4:G4)</f>
         <v>2</v>
       </c>
-      <c r="I4" s="137"/>
+      <c r="I4" s="138"/>
       <c r="J4" s="2"/>
       <c r="V4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="5" spans="2:22">
-      <c r="B5" s="82"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="135">
-        <v>1</v>
-      </c>
-      <c r="H5" s="136">
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="136">
+        <v>1</v>
+      </c>
+      <c r="H5" s="137">
         <f>SUM(D5:G5)</f>
         <v>1</v>
       </c>
-      <c r="I5" s="137"/>
+      <c r="I5" s="138"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="2:22">
@@ -3391,46 +3922,46 @@
       </c>
     </row>
     <row r="8" spans="2:22" ht="20" customHeight="1">
-      <c r="K8" s="122" t="s">
+      <c r="K8" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="119">
+      <c r="L8" s="120">
         <f>N8+N9+N10+P9+P10</f>
         <v>20</v>
       </c>
-      <c r="M8" s="77" t="s">
+      <c r="M8" s="150" t="s">
         <v>27</v>
       </c>
-      <c r="N8" s="124">
+      <c r="N8" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:22" ht="36" customHeight="1">
-      <c r="K9" s="122"/>
-      <c r="L9" s="120"/>
-      <c r="M9" s="78" t="s">
+      <c r="K9" s="123"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="N9" s="124">
-        <v>1</v>
-      </c>
-      <c r="O9" s="78" t="s">
+      <c r="N9" s="125">
+        <v>1</v>
+      </c>
+      <c r="O9" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="124">
+      <c r="P9" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:22" ht="25" customHeight="1">
-      <c r="K10" s="122"/>
-      <c r="L10" s="121"/>
-      <c r="M10" s="78"/>
-      <c r="N10" s="123">
+      <c r="K10" s="123"/>
+      <c r="L10" s="122"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="124">
         <f>P9+P10</f>
         <v>9</v>
       </c>
-      <c r="O10" s="78"/>
-      <c r="P10" s="123">
+      <c r="O10" s="142"/>
+      <c r="P10" s="124">
         <f>N12+N13+N15+N16+N17</f>
         <v>8</v>
       </c>
@@ -3442,44 +3973,44 @@
       </c>
     </row>
     <row r="12" spans="2:22">
-      <c r="K12" s="119" t="s">
-        <v>1</v>
-      </c>
-      <c r="L12" s="119">
+      <c r="K12" s="120" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="120">
         <f>N12+N13+P12+P13+R13</f>
         <v>5</v>
       </c>
-      <c r="M12" s="140" t="s">
+      <c r="M12" s="142" t="s">
         <v>30</v>
       </c>
-      <c r="N12" s="124">
-        <v>1</v>
-      </c>
-      <c r="O12" s="140" t="s">
+      <c r="N12" s="125">
+        <v>1</v>
+      </c>
+      <c r="O12" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="P12" s="127">
+      <c r="P12" s="128">
         <v>1</v>
       </c>
       <c r="Q12"/>
     </row>
     <row r="13" spans="2:22" ht="34" customHeight="1">
-      <c r="K13" s="121"/>
-      <c r="L13" s="121"/>
-      <c r="M13" s="140"/>
-      <c r="N13" s="123">
+      <c r="K13" s="122"/>
+      <c r="L13" s="122"/>
+      <c r="M13" s="142"/>
+      <c r="N13" s="124">
         <f>P12:P13</f>
         <v>1</v>
       </c>
-      <c r="O13" s="140"/>
-      <c r="P13" s="123">
+      <c r="O13" s="142"/>
+      <c r="P13" s="124">
         <f>R13</f>
         <v>1</v>
       </c>
       <c r="Q13" s="141" t="s">
         <v>32</v>
       </c>
-      <c r="R13" s="124">
+      <c r="R13" s="125">
         <v>1</v>
       </c>
     </row>
@@ -3490,146 +4021,146 @@
       </c>
     </row>
     <row r="15" spans="2:22" ht="20" customHeight="1">
-      <c r="K15" s="119" t="s">
+      <c r="K15" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="L15" s="119">
+      <c r="L15" s="120">
         <f>N15+N16+N17+P16+P17+P18</f>
         <v>10</v>
       </c>
       <c r="M15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="125">
+      <c r="N15" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:22" ht="20" customHeight="1">
-      <c r="K16" s="120"/>
-      <c r="L16" s="120"/>
-      <c r="M16" s="116" t="s">
+      <c r="K16" s="121"/>
+      <c r="L16" s="121"/>
+      <c r="M16" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="N16" s="125">
-        <v>1</v>
-      </c>
-      <c r="O16" s="75" t="s">
+      <c r="N16" s="126">
+        <v>1</v>
+      </c>
+      <c r="O16" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="P16" s="125">
+      <c r="P16" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="11:20" ht="20" customHeight="1">
-      <c r="K17" s="120"/>
-      <c r="L17" s="120"/>
-      <c r="M17" s="117"/>
-      <c r="N17" s="108">
+      <c r="K17" s="121"/>
+      <c r="L17" s="121"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="109">
         <f>P16+P17+P18</f>
         <v>4</v>
       </c>
-      <c r="O17" s="145" t="s">
+      <c r="O17" s="143" t="s">
         <v>128</v>
       </c>
-      <c r="P17" s="126">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="138" t="s">
+      <c r="P17" s="127">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="R17" s="138">
+      <c r="R17" s="139">
         <f>T17+T18</f>
         <v>2</v>
       </c>
-      <c r="S17" s="124" t="s">
+      <c r="S17" s="145" t="s">
         <v>126</v>
       </c>
-      <c r="T17" s="125">
+      <c r="T17" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="11:20" ht="20" customHeight="1">
-      <c r="K18" s="121"/>
-      <c r="L18" s="121"/>
-      <c r="M18" s="118"/>
-      <c r="N18" s="109"/>
-      <c r="O18" s="146"/>
-      <c r="P18" s="123">
+      <c r="K18" s="122"/>
+      <c r="L18" s="122"/>
+      <c r="M18" s="119"/>
+      <c r="N18" s="110"/>
+      <c r="O18" s="144"/>
+      <c r="P18" s="124">
         <f>R17</f>
         <v>2</v>
       </c>
-      <c r="Q18" s="139"/>
-      <c r="R18" s="139"/>
-      <c r="S18" s="124" t="s">
+      <c r="Q18" s="140"/>
+      <c r="R18" s="140"/>
+      <c r="S18" s="145" t="s">
         <v>127</v>
       </c>
-      <c r="T18" s="125">
+      <c r="T18" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="11:20">
-      <c r="K19" s="130">
+      <c r="K19" s="131">
         <f>L20/3</f>
         <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="20" spans="11:20" ht="20" customHeight="1">
-      <c r="K20" s="119" t="s">
+      <c r="K20" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="L20" s="119">
+      <c r="L20" s="120">
         <f>N21+N20</f>
         <v>5</v>
       </c>
-      <c r="M20" s="142" t="s">
+      <c r="M20" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="N20" s="124">
-        <v>1</v>
-      </c>
-      <c r="O20" s="114" t="s">
+      <c r="N20" s="125">
+        <v>1</v>
+      </c>
+      <c r="O20" s="151" t="s">
         <v>38</v>
       </c>
-      <c r="P20" s="124">
+      <c r="P20" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="11:20" ht="20" customHeight="1">
-      <c r="K21" s="120"/>
-      <c r="L21" s="120"/>
-      <c r="M21" s="143"/>
-      <c r="N21" s="119">
+      <c r="K21" s="121"/>
+      <c r="L21" s="121"/>
+      <c r="M21" s="147"/>
+      <c r="N21" s="120">
         <f>P20+P21+P22+P23</f>
         <v>4</v>
       </c>
-      <c r="O21" s="114" t="s">
+      <c r="O21" s="151" t="s">
         <v>39</v>
       </c>
-      <c r="P21" s="124">
+      <c r="P21" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="11:20" ht="20" customHeight="1">
-      <c r="K22" s="120"/>
-      <c r="L22" s="120"/>
-      <c r="M22" s="143"/>
-      <c r="N22" s="120"/>
-      <c r="O22" s="114" t="s">
+      <c r="K22" s="121"/>
+      <c r="L22" s="121"/>
+      <c r="M22" s="147"/>
+      <c r="N22" s="121"/>
+      <c r="O22" s="151" t="s">
         <v>40</v>
       </c>
-      <c r="P22" s="124">
+      <c r="P22" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="11:20" ht="20" customHeight="1">
-      <c r="K23" s="121"/>
-      <c r="L23" s="121"/>
-      <c r="M23" s="144"/>
-      <c r="N23" s="121"/>
-      <c r="O23" s="114" t="s">
+      <c r="K23" s="122"/>
+      <c r="L23" s="122"/>
+      <c r="M23" s="148"/>
+      <c r="N23" s="122"/>
+      <c r="O23" s="151" t="s">
         <v>41</v>
       </c>
-      <c r="P23" s="124">
+      <c r="P23" s="125">
         <v>1</v>
       </c>
     </row>
@@ -3656,430 +4187,6 @@
     <mergeCell ref="I3:I5"/>
     <mergeCell ref="K8:K10"/>
     <mergeCell ref="L8:L10"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H50"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4" style="1" customWidth="1"/>
-    <col min="4" max="4" width="64.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="65.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:8">
-      <c r="C3" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="C5" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" t="s">
-        <v>179</v>
-      </c>
-      <c r="F5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" t="s">
-        <v>172</v>
-      </c>
-      <c r="F6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="1">
-        <f>C6+1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>139</v>
-      </c>
-      <c r="B8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C8" s="1">
-        <f t="shared" ref="C8:C14" si="0">C7+1</f>
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E8" t="s">
-        <v>172</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="C9" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E9" t="s">
-        <v>172</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="C10" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>173</v>
-      </c>
-      <c r="E10" t="s">
-        <v>172</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="C11" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="C12" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="E12" t="s">
-        <v>172</v>
-      </c>
-      <c r="F12">
-        <v>0.5</v>
-      </c>
-      <c r="G12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>146</v>
-      </c>
-      <c r="E15" t="s">
-        <v>172</v>
-      </c>
-      <c r="F15">
-        <v>0.5</v>
-      </c>
-      <c r="G15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="D16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="D18" t="s">
-        <v>176</v>
-      </c>
-      <c r="E18" t="s">
-        <v>172</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="D19" t="s">
-        <v>175</v>
-      </c>
-      <c r="E19" t="s">
-        <v>172</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>140</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>152</v>
-      </c>
-      <c r="E21" t="s">
-        <v>170</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="D22" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="D23" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="D24" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="D26" t="s">
-        <v>180</v>
-      </c>
-      <c r="E26" t="s">
-        <v>172</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="C29" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="C30" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="s">
-        <v>138</v>
-      </c>
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="s">
-        <v>139</v>
-      </c>
-      <c r="D32" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>140</v>
-      </c>
-      <c r="D33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="D34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>138</v>
-      </c>
-      <c r="B35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>137</v>
-      </c>
-      <c r="D36" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="D38" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="D41" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="D43" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="D44" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="D45" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="D47" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="D48" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4">
-      <c r="D49" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4">
-      <c r="D50" t="s">
-        <v>164</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C29:H29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4234,71 +4341,71 @@
     </row>
     <row r="3" spans="2:8" ht="24" customHeight="1">
       <c r="B3" s="33"/>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="79" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
       <c r="H3" s="33"/>
     </row>
     <row r="4" spans="2:8" ht="27" customHeight="1">
       <c r="B4" s="35"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="84" t="s">
+      <c r="C4" s="79"/>
+      <c r="D4" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="77" t="s">
+      <c r="E4" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="78" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="33"/>
     </row>
     <row r="5" spans="2:8" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="B5" s="34"/>
-      <c r="C5" s="86" t="s">
+      <c r="C5" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="87" t="s">
+      <c r="D5" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="88" t="s">
+      <c r="E5" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="88" t="s">
+      <c r="F5" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="89" t="s">
+      <c r="G5" s="90" t="s">
         <v>50</v>
       </c>
       <c r="H5" s="34"/>
     </row>
     <row r="6" spans="2:8" ht="20" customHeight="1">
       <c r="B6" s="35"/>
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="91"/>
-      <c r="G6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="93"/>
       <c r="H6" s="33"/>
     </row>
     <row r="7" spans="2:8" ht="20" customHeight="1">
       <c r="B7" s="35"/>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="84" t="s">
         <v>56</v>
       </c>
       <c r="D7" s="6"/>
@@ -4313,22 +4420,22 @@
     </row>
     <row r="8" spans="2:8" ht="20" customHeight="1">
       <c r="B8" s="33"/>
-      <c r="C8" s="85" t="s">
+      <c r="C8" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="90"/>
-      <c r="E8" s="91" t="s">
+      <c r="D8" s="91"/>
+      <c r="E8" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="91" t="s">
+      <c r="F8" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="92"/>
+      <c r="G8" s="93"/>
       <c r="H8" s="33"/>
     </row>
     <row r="9" spans="2:8" ht="20" customHeight="1">
       <c r="B9" s="33"/>
-      <c r="C9" s="83" t="s">
+      <c r="C9" s="84" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -4343,24 +4450,24 @@
     </row>
     <row r="10" spans="2:8" ht="20" customHeight="1">
       <c r="B10" s="33"/>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="90"/>
-      <c r="E10" s="91" t="s">
+      <c r="D10" s="91"/>
+      <c r="E10" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="91" t="s">
+      <c r="F10" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="92" t="s">
+      <c r="G10" s="93" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="33"/>
     </row>
     <row r="11" spans="2:8" ht="20" customHeight="1">
       <c r="B11" s="33"/>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="84" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -4377,14 +4484,14 @@
     </row>
     <row r="12" spans="2:8" ht="20" customHeight="1">
       <c r="B12" s="33"/>
-      <c r="C12" s="85" t="s">
+      <c r="C12" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="90"/>
-      <c r="E12" s="91" t="s">
+      <c r="D12" s="91"/>
+      <c r="E12" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="91"/>
+      <c r="F12" s="92"/>
       <c r="G12" s="9" t="s">
         <v>62</v>
       </c>
@@ -4392,7 +4499,7 @@
     </row>
     <row r="13" spans="2:8" ht="20" customHeight="1">
       <c r="B13" s="33"/>
-      <c r="C13" s="83" t="s">
+      <c r="C13" s="84" t="s">
         <v>54</v>
       </c>
       <c r="D13" s="10"/>
@@ -4514,124 +4621,124 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="33"/>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
       <c r="G3" s="33"/>
     </row>
     <row r="4" spans="1:7" ht="25" customHeight="1">
       <c r="A4" s="33"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="53"/>
+      <c r="C4" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="54" t="s">
+      <c r="D4" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="55" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A5" s="34"/>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="66" t="s">
+      <c r="C5" s="65"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="67"/>
+      <c r="F5" s="68"/>
       <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A6" s="34"/>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="57" t="s">
+      <c r="C6" s="57"/>
+      <c r="D6" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F6" s="59" t="s">
         <v>66</v>
       </c>
       <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A7" s="34"/>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="69" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="70"/>
-      <c r="F7" s="51"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A8" s="34"/>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="57" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="60" t="s">
         <v>50</v>
       </c>
       <c r="G8" s="34"/>
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A9" s="34"/>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50" t="s">
+      <c r="C9" s="50"/>
+      <c r="D9" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="50" t="s">
+      <c r="E9" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="52" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A10" s="34"/>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61" t="s">
+      <c r="C10" s="61"/>
+      <c r="D10" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="62" t="s">
+      <c r="E10" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="64" t="s">
         <v>50</v>
       </c>
       <c r="G10" s="34"/>
@@ -4711,353 +4818,353 @@
     </row>
     <row r="2" spans="1:15" ht="22" customHeight="1">
       <c r="A2" s="33"/>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="83" t="s">
         <v>110</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
       <c r="M2" s="33"/>
       <c r="N2" s="24"/>
     </row>
     <row r="3" spans="1:15" ht="39" customHeight="1">
       <c r="A3" s="33"/>
-      <c r="B3" s="82"/>
-      <c r="C3" s="81" t="s">
+      <c r="B3" s="83"/>
+      <c r="C3" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="79" t="s">
+      <c r="F3" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="75" t="s">
+      <c r="G3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="75" t="s">
+      <c r="H3" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="80" t="s">
+      <c r="I3" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="75" t="s">
+      <c r="J3" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="79" t="s">
+      <c r="K3" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="75" t="s">
+      <c r="L3" s="76" t="s">
         <v>94</v>
       </c>
       <c r="M3" s="35"/>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1">
       <c r="A4" s="33"/>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93" t="s">
+      <c r="F4" s="94"/>
+      <c r="G4" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93" t="s">
+      <c r="H4" s="94"/>
+      <c r="I4" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="94" t="s">
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="95" t="s">
         <v>10</v>
       </c>
       <c r="M4" s="33"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1">
       <c r="A5" s="33"/>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="95"/>
-      <c r="L5" s="96" t="s">
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="97" t="s">
         <v>10</v>
       </c>
       <c r="M5" s="33"/>
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1">
       <c r="A6" s="33"/>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="93" t="s">
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93" t="s">
+      <c r="H6" s="94"/>
+      <c r="I6" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="94" t="s">
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="95" t="s">
         <v>10</v>
       </c>
       <c r="M6" s="33"/>
     </row>
     <row r="7" spans="1:15" ht="30">
       <c r="A7" s="33"/>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="95" t="s">
+      <c r="D7" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="95"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="98" t="s">
+      <c r="E7" s="96"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="98" t="s">
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="98" t="s">
+      <c r="K7" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="100"/>
+      <c r="L7" s="101"/>
       <c r="M7" s="33"/>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1">
       <c r="A8" s="33"/>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93" t="s">
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="97"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="94" t="s">
+      <c r="F8" s="98"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="95" t="s">
         <v>10</v>
       </c>
       <c r="M8" s="33"/>
     </row>
     <row r="9" spans="1:15" ht="30">
       <c r="A9" s="33"/>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="95" t="s">
+      <c r="D9" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="95" t="s">
+      <c r="E9" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="95" t="s">
+      <c r="F9" s="96" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="95"/>
-      <c r="H9" s="95" t="s">
+      <c r="G9" s="96"/>
+      <c r="H9" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95" t="s">
+      <c r="I9" s="96"/>
+      <c r="J9" s="96" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="95" t="s">
+      <c r="K9" s="96" t="s">
         <v>92</v>
       </c>
-      <c r="L9" s="98" t="s">
+      <c r="L9" s="99" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="33"/>
     </row>
     <row r="10" spans="1:15" ht="30" customHeight="1">
       <c r="A10" s="33"/>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93"/>
-      <c r="E10" s="93"/>
-      <c r="F10" s="93"/>
-      <c r="G10" s="93"/>
-      <c r="H10" s="93" t="s">
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93" t="s">
+      <c r="I10" s="94"/>
+      <c r="J10" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="K10" s="93"/>
-      <c r="L10" s="94" t="s">
+      <c r="K10" s="94"/>
+      <c r="L10" s="95" t="s">
         <v>10</v>
       </c>
       <c r="M10" s="33"/>
     </row>
     <row r="11" spans="1:15" ht="30">
       <c r="A11" s="33"/>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="98" t="s">
+      <c r="D11" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="100"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="96"/>
+      <c r="J11" s="96"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="101"/>
       <c r="M11" s="33"/>
     </row>
     <row r="12" spans="1:15" ht="30" customHeight="1">
       <c r="A12" s="33"/>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="93"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="94" t="s">
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="93"/>
-      <c r="J12" s="93"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="101"/>
+      <c r="I12" s="94"/>
+      <c r="J12" s="94"/>
+      <c r="K12" s="94"/>
+      <c r="L12" s="102"/>
       <c r="M12" s="33"/>
     </row>
     <row r="13" spans="1:15" ht="30">
       <c r="A13" s="33"/>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="95" t="s">
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="95" t="s">
+      <c r="G13" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="H13" s="95"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="95"/>
-      <c r="K13" s="95"/>
-      <c r="L13" s="98" t="s">
+      <c r="H13" s="96"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="96"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="99" t="s">
         <v>10</v>
       </c>
       <c r="M13" s="33"/>
     </row>
     <row r="14" spans="1:15" ht="37" customHeight="1">
       <c r="A14" s="33"/>
-      <c r="B14" s="83" t="s">
+      <c r="B14" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93" t="s">
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="93"/>
-      <c r="K14" s="93" t="s">
+      <c r="J14" s="94"/>
+      <c r="K14" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="L14" s="93" t="s">
+      <c r="L14" s="94" t="s">
         <v>93</v>
       </c>
       <c r="M14" s="33"/>
     </row>
     <row r="15" spans="1:15" ht="30" customHeight="1">
       <c r="A15" s="33"/>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="102"/>
-      <c r="L15" s="95"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="100"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="96"/>
       <c r="M15" s="33"/>
       <c r="O15" s="24"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1">
       <c r="A16" s="33"/>
-      <c r="B16" s="83" t="s">
+      <c r="B16" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="93"/>
-      <c r="K16" s="97"/>
-      <c r="L16" s="94" t="s">
+      <c r="C16" s="94"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="95" t="s">
         <v>10</v>
       </c>
       <c r="M16" s="33"/>
@@ -5065,43 +5172,43 @@
     </row>
     <row r="17" spans="1:15" ht="30">
       <c r="A17" s="33"/>
-      <c r="B17" s="77" t="s">
+      <c r="B17" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95" t="s">
+      <c r="C17" s="96"/>
+      <c r="D17" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="99"/>
-      <c r="I17" s="98" t="s">
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="100"/>
+      <c r="I17" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="J17" s="95"/>
-      <c r="K17" s="99" t="s">
+      <c r="J17" s="96"/>
+      <c r="K17" s="100" t="s">
         <v>109</v>
       </c>
-      <c r="L17" s="95"/>
+      <c r="L17" s="96"/>
       <c r="M17" s="33"/>
       <c r="O17" s="24"/>
     </row>
     <row r="18" spans="1:15" ht="30" customHeight="1">
       <c r="A18" s="33"/>
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="97"/>
-      <c r="I18" s="93"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="97"/>
-      <c r="L18" s="94" t="s">
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="98"/>
+      <c r="L18" s="95" t="s">
         <v>10</v>
       </c>
       <c r="M18" s="33"/>
@@ -5109,19 +5216,19 @@
     </row>
     <row r="19" spans="1:15" ht="30" customHeight="1">
       <c r="A19" s="33"/>
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="95"/>
-      <c r="G19" s="95"/>
-      <c r="H19" s="99"/>
-      <c r="I19" s="95"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="99"/>
-      <c r="L19" s="100" t="s">
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="100"/>
+      <c r="I19" s="96"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="100"/>
+      <c r="L19" s="101" t="s">
         <v>10</v>
       </c>
       <c r="M19" s="33"/>
@@ -5183,9 +5290,9 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
       <c r="J7" s="3" t="s">
         <v>101</v>
       </c>
@@ -5211,116 +5318,116 @@
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="73" t="s">
+      <c r="D9" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
       <c r="H9" s="46" t="s">
         <v>97</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="74"/>
+      <c r="J9" s="75"/>
     </row>
     <row r="10" spans="2:14" ht="18">
       <c r="B10" s="46"/>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="74" t="s">
+      <c r="D10" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
       <c r="H10" s="46"/>
       <c r="I10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="74"/>
+      <c r="J10" s="75"/>
     </row>
     <row r="11" spans="2:14" ht="18">
       <c r="B11" s="46"/>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
       <c r="H11" s="46"/>
       <c r="I11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="74"/>
+      <c r="J11" s="75"/>
     </row>
     <row r="12" spans="2:14" ht="18">
       <c r="B12" s="46"/>
       <c r="C12" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="74" t="s">
+      <c r="D12" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="74"/>
+      <c r="F12" s="75"/>
       <c r="H12" s="46"/>
       <c r="I12" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="74"/>
+      <c r="J12" s="75"/>
     </row>
     <row r="13" spans="2:14" ht="18">
       <c r="B13" s="46" t="s">
         <v>96</v>
       </c>
       <c r="C13" s="43"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74" t="s">
+      <c r="D13" s="75"/>
+      <c r="E13" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="74"/>
+      <c r="F13" s="75"/>
       <c r="H13" s="46" t="s">
         <v>96</v>
       </c>
       <c r="I13" s="43"/>
-      <c r="J13" s="74"/>
+      <c r="J13" s="75"/>
     </row>
     <row r="14" spans="2:14" ht="18">
       <c r="B14" s="46"/>
       <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74" t="s">
+      <c r="D14" s="75"/>
+      <c r="E14" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="74"/>
+      <c r="F14" s="75"/>
       <c r="H14" s="46"/>
       <c r="I14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="74"/>
+      <c r="J14" s="75"/>
     </row>
     <row r="15" spans="2:14" ht="18">
       <c r="B15" s="46"/>
       <c r="C15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74" t="s">
+      <c r="D15" s="75"/>
+      <c r="E15" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="74"/>
+      <c r="F15" s="75"/>
       <c r="H15" s="46"/>
       <c r="I15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J15" s="74"/>
+      <c r="J15" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5359,22 +5466,22 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:5" ht="114" customHeight="1">
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="77" t="s">
+      <c r="D5" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="76" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="80" customHeight="1">
-      <c r="C6" s="76"/>
-      <c r="D6" s="77" t="s">
+      <c r="C6" s="77"/>
+      <c r="D6" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="E6" s="75" t="s">
+      <c r="E6" s="76" t="s">
         <v>103</v>
       </c>
     </row>
@@ -5460,7 +5567,7 @@
       <c r="B7" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="103" t="s">
+      <c r="C7" s="104" t="s">
         <v>123</v>
       </c>
     </row>
@@ -5491,7 +5598,7 @@
     <col min="5" max="5" width="3.83203125" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="113" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="114" customWidth="1"/>
     <col min="9" max="9" width="3.83203125" customWidth="1"/>
     <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.83203125" customWidth="1"/>
@@ -5508,227 +5615,227 @@
       </c>
     </row>
     <row r="7" spans="2:13" ht="20" customHeight="1">
-      <c r="B7" s="122" t="s">
+      <c r="B7" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="119">
+      <c r="C7" s="120">
         <f>E7+E8+E9+G8+G9</f>
         <v>20</v>
       </c>
-      <c r="D7" s="77" t="s">
+      <c r="D7" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="124">
+      <c r="E7" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="122"/>
-      <c r="C8" s="120"/>
-      <c r="D8" s="78" t="s">
+      <c r="B8" s="123"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="124">
-        <v>1</v>
-      </c>
-      <c r="F8" s="78" t="s">
+      <c r="E8" s="125">
+        <v>1</v>
+      </c>
+      <c r="F8" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="124">
+      <c r="G8" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="122"/>
-      <c r="C9" s="121"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="129">
+      <c r="B9" s="123"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="130">
         <f>G8+G9</f>
         <v>9</v>
       </c>
-      <c r="F9" s="78"/>
-      <c r="G9" s="123">
+      <c r="F9" s="79"/>
+      <c r="G9" s="124">
         <f>E11+E12+E14+E15+E16</f>
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:13">
-      <c r="B11" s="119" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="119">
+      <c r="B11" s="120" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="120">
         <f>E11+E12+G11+G12+I12</f>
         <v>5</v>
       </c>
-      <c r="D11" s="78" t="s">
+      <c r="D11" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="124">
-        <v>1</v>
-      </c>
-      <c r="F11" s="78" t="s">
+      <c r="E11" s="125">
+        <v>1</v>
+      </c>
+      <c r="F11" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="127">
+      <c r="G11" s="128">
         <v>1</v>
       </c>
       <c r="H11"/>
     </row>
     <row r="12" spans="2:13" ht="38" customHeight="1">
-      <c r="B12" s="121"/>
-      <c r="C12" s="121"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="123">
+      <c r="B12" s="122"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="124">
         <f>G11:G12</f>
         <v>1</v>
       </c>
-      <c r="F12" s="78"/>
-      <c r="G12" s="123">
+      <c r="F12" s="79"/>
+      <c r="G12" s="124">
         <f>I12</f>
         <v>1</v>
       </c>
-      <c r="H12" s="81" t="s">
+      <c r="H12" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="124">
+      <c r="I12" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="20" customHeight="1">
-      <c r="B14" s="122" t="s">
+      <c r="B14" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="119">
+      <c r="C14" s="120">
         <f>E14+E15+E16+G15+G16+G17</f>
         <v>10</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="125">
+      <c r="E14" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="36" customHeight="1">
-      <c r="B15" s="122"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="78" t="s">
+      <c r="B15" s="123"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="128">
-        <v>1</v>
-      </c>
-      <c r="F15" s="75" t="s">
+      <c r="E15" s="129">
+        <v>1</v>
+      </c>
+      <c r="F15" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="125">
+      <c r="G15" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="25" customHeight="1">
-      <c r="B16" s="122"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="108">
+      <c r="B16" s="123"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="109">
         <f>G15+G16+G17</f>
         <v>4</v>
       </c>
-      <c r="F16" s="82" t="s">
+      <c r="F16" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="G16" s="126">
-        <v>1</v>
-      </c>
-      <c r="H16" s="82" t="s">
+      <c r="G16" s="127">
+        <v>1</v>
+      </c>
+      <c r="H16" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="82">
+      <c r="I16" s="83">
         <f>K16+K17</f>
         <v>2</v>
       </c>
-      <c r="J16" s="115" t="s">
+      <c r="J16" s="116" t="s">
         <v>126</v>
       </c>
-      <c r="K16" s="125">
+      <c r="K16" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="25" customHeight="1">
-      <c r="B17" s="122"/>
-      <c r="C17" s="121"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="123">
+      <c r="B17" s="123"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="124">
         <f>I16</f>
         <v>2</v>
       </c>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="115" t="s">
+      <c r="H17" s="83"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="116" t="s">
         <v>127</v>
       </c>
-      <c r="K17" s="125">
+      <c r="K17" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:11" ht="20" customHeight="1">
-      <c r="B19" s="122" t="s">
+      <c r="B19" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="122">
+      <c r="C19" s="123">
         <f>E20+E19</f>
         <v>5</v>
       </c>
-      <c r="D19" s="78" t="s">
+      <c r="D19" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="124">
-        <v>1</v>
-      </c>
-      <c r="F19" s="114" t="s">
+      <c r="E19" s="125">
+        <v>1</v>
+      </c>
+      <c r="F19" s="115" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="124">
+      <c r="G19" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="20" customHeight="1">
-      <c r="B20" s="122"/>
-      <c r="C20" s="122"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="119">
+      <c r="B20" s="123"/>
+      <c r="C20" s="123"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="120">
         <f>G19+G20+G21+G22</f>
         <v>4</v>
       </c>
-      <c r="F20" s="114" t="s">
+      <c r="F20" s="115" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="124">
+      <c r="G20" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="20" customHeight="1">
-      <c r="B21" s="122"/>
-      <c r="C21" s="122"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="114" t="s">
+      <c r="B21" s="123"/>
+      <c r="C21" s="123"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="121"/>
+      <c r="F21" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="124">
+      <c r="G21" s="125">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:11" ht="20" customHeight="1">
-      <c r="B22" s="122"/>
-      <c r="C22" s="122"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="121"/>
-      <c r="F22" s="114" t="s">
+      <c r="B22" s="123"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="122"/>
+      <c r="F22" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="124">
+      <c r="G22" s="125">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added pending saved changes on previous commit
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-820" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="500" firstSheet="10" activeTab="11"/>
+    <workbookView xWindow="-820" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="500" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7306,7 +7306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -8716,7 +8716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added and deleted important changes.
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" activeTab="1"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="25360" windowHeight="15280" firstSheet="11" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="227">
   <si>
     <t>ACCESSIBILITY</t>
   </si>
@@ -804,6 +804,27 @@
   </si>
   <si>
     <t>H4.6.4</t>
+  </si>
+  <si>
+    <t>Was the service interrupted when you were using it (not because Internet connection)?</t>
+  </si>
+  <si>
+    <t>Do you consider the e-service as useful?</t>
+  </si>
+  <si>
+    <t>Do you consider the service functionality as reliable?</t>
+  </si>
+  <si>
+    <t>Was the graphic interface comprehensive?</t>
+  </si>
+  <si>
+    <t>Were you informed on how to contact provider in case needing help?</t>
+  </si>
+  <si>
+    <t>Was the service provider responsive?</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1458,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="368">
+  <cellStyleXfs count="370">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1798,6 +1819,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2594,7 +2617,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="368">
+  <cellStyles count="370">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2778,6 +2801,7 @@
     <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2961,6 +2985,7 @@
     <cellStyle name="Hyperlink" xfId="362" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="359" builtinId="5"/>
   </cellStyles>
@@ -5156,7 +5181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -5209,12 +5234,12 @@
       <c r="F3" s="223"/>
       <c r="G3" s="224">
         <f>E10/4</f>
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="H3" s="224"/>
       <c r="I3" s="224">
         <f>E14/2</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="J3" s="224"/>
       <c r="K3" s="224">
@@ -5224,7 +5249,7 @@
       <c r="L3" s="224"/>
       <c r="M3" s="225">
         <f>E22/3</f>
-        <v>3</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="N3" s="226"/>
       <c r="O3" s="227" t="s">
@@ -5268,7 +5293,7 @@
       <c r="B5" s="134"/>
       <c r="C5" s="263">
         <f>(G5+K5+G6+K6+M7+I5)/O5</f>
-        <v>1</v>
+        <v>0.71666666666666667</v>
       </c>
       <c r="D5" s="215" t="s">
         <v>121</v>
@@ -5279,12 +5304,12 @@
       <c r="F5" s="208"/>
       <c r="G5" s="168">
         <f>G3</f>
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="H5" s="168"/>
       <c r="I5" s="209">
         <f>I3</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="J5" s="209"/>
       <c r="K5" s="168">
@@ -5297,7 +5322,6 @@
       </c>
       <c r="N5" s="219"/>
       <c r="O5" s="205">
-        <f>(G5+K5+G6+K6+M7+I5)</f>
         <v>20</v>
       </c>
       <c r="P5" s="135"/>
@@ -5312,7 +5336,7 @@
       <c r="F6" s="208"/>
       <c r="G6" s="209">
         <f>G3</f>
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="H6" s="209" t="str">
         <f>$D$9</f>
@@ -5361,7 +5385,7 @@
       <c r="L7" s="210"/>
       <c r="M7" s="190">
         <f>M3</f>
-        <v>3</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="N7" s="220"/>
       <c r="O7" s="206"/>
@@ -5430,7 +5454,7 @@
       </c>
       <c r="E10" s="176">
         <f>G10+G11+G12+I11+I12</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F10" s="70" t="s">
         <v>27</v>
@@ -5459,7 +5483,7 @@
       </c>
       <c r="G11" s="156">
         <f>Users_Survey!E6+Users_Survey!E7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="168" t="s">
         <v>29</v>
@@ -5484,12 +5508,12 @@
       <c r="F12" s="168"/>
       <c r="G12" s="157">
         <f>I11+I12</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H12" s="168"/>
       <c r="I12" s="157">
         <f>G14+G15+G17+G18+G19</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J12" s="137"/>
       <c r="K12" s="136"/>
@@ -5526,7 +5550,7 @@
       </c>
       <c r="E14" s="176">
         <f>G14+G15+I14+I15+K15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F14" s="168" t="s">
         <v>30</v>
@@ -5540,7 +5564,7 @@
       </c>
       <c r="I14" s="156">
         <f>Users_Survey!E10</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="136"/>
       <c r="K14" s="136"/>
@@ -5558,19 +5582,19 @@
       <c r="F15" s="168"/>
       <c r="G15" s="157">
         <f>I14+I15</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="168"/>
       <c r="I15" s="157">
         <f>K15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="74" t="s">
         <v>32</v>
       </c>
       <c r="K15" s="156">
         <f>Users_Survey!E11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="136"/>
       <c r="M15" s="136"/>
@@ -5633,7 +5657,7 @@
         <v>34</v>
       </c>
       <c r="G18" s="156">
-        <f>Users_Survey!E13</f>
+        <f>Users_Survey!E13+Users_Survey!E14</f>
         <v>1</v>
       </c>
       <c r="H18" s="86"/>
@@ -5660,7 +5684,7 @@
         <v>125</v>
       </c>
       <c r="I19" s="193">
-        <f>Users_Survey!E14+Users_Survey!E15</f>
+        <f>Users_Survey!E15+Users_Survey!E16</f>
         <v>1</v>
       </c>
       <c r="J19" s="181" t="s">
@@ -5671,7 +5695,7 @@
       </c>
       <c r="L19" s="168"/>
       <c r="M19" s="156">
-        <f>Users_Survey!E16</f>
+        <f>Users_Survey!E17</f>
         <v>1</v>
       </c>
       <c r="N19" s="136"/>
@@ -5693,7 +5717,7 @@
       </c>
       <c r="L20" s="168"/>
       <c r="M20" s="156">
-        <f>Users_Survey!E17</f>
+        <f>Users_Survey!E18</f>
         <v>1</v>
       </c>
       <c r="N20" s="136"/>
@@ -5727,20 +5751,20 @@
       </c>
       <c r="E22" s="176">
         <f>G23+G22+I22+I23+I24+I25</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F22" s="182" t="s">
         <v>37</v>
       </c>
       <c r="G22" s="156">
-        <f>Users_Survey!E18</f>
+        <f>Users_Survey!E19</f>
         <v>1</v>
       </c>
       <c r="H22" s="106" t="s">
         <v>38</v>
       </c>
       <c r="I22" s="156">
-        <f>Users_Survey!E19</f>
+        <f>Users_Survey!E20</f>
         <v>1</v>
       </c>
       <c r="J22" s="137"/>
@@ -5759,14 +5783,14 @@
       <c r="F23" s="183"/>
       <c r="G23" s="200">
         <f>I22+I23+I24+I25</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H23" s="106" t="s">
         <v>39</v>
       </c>
       <c r="I23" s="156">
-        <f>Users_Survey!E20</f>
-        <v>1</v>
+        <f>Users_Survey!E21</f>
+        <v>0</v>
       </c>
       <c r="J23" s="137"/>
       <c r="K23" s="136"/>
@@ -5787,7 +5811,7 @@
         <v>40</v>
       </c>
       <c r="I24" s="156">
-        <f>Users_Survey!E21</f>
+        <f>Users_Survey!E22</f>
         <v>1</v>
       </c>
       <c r="J24" s="137"/>
@@ -5809,7 +5833,7 @@
         <v>41</v>
       </c>
       <c r="I25" s="156">
-        <f>Users_Survey!E22</f>
+        <f>Users_Survey!E23</f>
         <v>1</v>
       </c>
       <c r="J25" s="137"/>
@@ -5847,7 +5871,7 @@
       </c>
       <c r="E27" s="191">
         <f>G10+G17+M7+G22+I24+I25</f>
-        <v>8</v>
+        <v>7.3333333333333339</v>
       </c>
       <c r="F27" s="192"/>
       <c r="G27" s="136"/>
@@ -6086,7 +6110,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6142,13 +6166,13 @@
     </row>
     <row r="4" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="230"/>
-      <c r="B4" s="70">
+      <c r="B4" s="71">
         <v>1</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="71" t="s">
         <v>166</v>
       </c>
       <c r="E4" s="107">
@@ -6162,14 +6186,14 @@
     </row>
     <row r="5" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="230"/>
-      <c r="B5" s="70">
+      <c r="B5" s="71">
         <f>B4+1</f>
         <v>2</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="71" t="s">
         <v>166</v>
       </c>
       <c r="E5" s="107">
@@ -6183,19 +6207,19 @@
     </row>
     <row r="6" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="230"/>
-      <c r="B6" s="70">
-        <f t="shared" ref="B6:B22" si="1">B5+1</f>
+      <c r="B6" s="71">
+        <f t="shared" ref="B6:B23" si="1">B5+1</f>
         <v>3</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D6" s="70" t="s">
-        <v>166</v>
+      <c r="C6" s="160" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" s="71" t="s">
+        <v>143</v>
       </c>
       <c r="E6" s="107">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>28</v>
@@ -6204,19 +6228,17 @@
     </row>
     <row r="7" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="230"/>
-      <c r="B7" s="70">
+      <c r="B7" s="71">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C7" s="160" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" s="70" t="s">
-        <v>166</v>
-      </c>
+      <c r="C7" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" s="71"/>
       <c r="E7" s="107">
         <f>IF(D7="YES",0.5,0)</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>28</v>
@@ -6225,14 +6247,14 @@
     </row>
     <row r="8" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="230"/>
-      <c r="B8" s="70">
+      <c r="B8" s="71">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="D8" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" s="71" t="s">
         <v>143</v>
       </c>
       <c r="E8" s="107">
@@ -6246,14 +6268,14 @@
     </row>
     <row r="9" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="230"/>
-      <c r="B9" s="70">
+      <c r="B9" s="71">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="71" t="s">
         <v>166</v>
       </c>
       <c r="E9" s="107">
@@ -6267,19 +6289,17 @@
     </row>
     <row r="10" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="230"/>
-      <c r="B10" s="70">
+      <c r="B10" s="71">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D10" s="70" t="s">
-        <v>166</v>
-      </c>
+      <c r="D10" s="71"/>
       <c r="E10" s="107">
         <f>IF(D10="YES",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>31</v>
@@ -6288,19 +6308,17 @@
     </row>
     <row r="11" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="230"/>
-      <c r="B11" s="70">
+      <c r="B11" s="71">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="D11" s="70" t="s">
-        <v>166</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="D11" s="71"/>
       <c r="E11" s="107">
         <f>IF(D11="YES",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>32</v>
@@ -6309,14 +6327,14 @@
     </row>
     <row r="12" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="230"/>
-      <c r="B12" s="70">
+      <c r="B12" s="71">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="71" t="s">
         <v>143</v>
       </c>
       <c r="E12" s="107">
@@ -6330,19 +6348,19 @@
     </row>
     <row r="13" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="230"/>
-      <c r="B13" s="70">
+      <c r="B13" s="71">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="D13" s="70" t="s">
+      <c r="C13" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" s="71" t="s">
         <v>166</v>
       </c>
       <c r="E13" s="107">
-        <f>IF(D13="YES",1,0)</f>
-        <v>1</v>
+        <f>IF(D13="YES",0.5,0)</f>
+        <v>0.5</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>34</v>
@@ -6351,35 +6369,35 @@
     </row>
     <row r="14" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="230"/>
-      <c r="B14" s="70">
+      <c r="B14" s="71">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C14" s="161" t="s">
-        <v>137</v>
-      </c>
-      <c r="D14" s="70" t="s">
-        <v>166</v>
+      <c r="C14" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D14" s="71" t="s">
+        <v>226</v>
       </c>
       <c r="E14" s="107">
-        <f>IF(D14="YES",0.5,0)</f>
+        <f>IF(D14="NO",0,0.5)</f>
         <v>0.5</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>125</v>
+        <v>34</v>
       </c>
       <c r="G14" s="230"/>
     </row>
     <row r="15" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A15" s="230"/>
-      <c r="B15" s="70">
+      <c r="B15" s="71">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D15" s="70" t="s">
+      <c r="C15" s="161" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="71" t="s">
         <v>166</v>
       </c>
       <c r="E15" s="107">
@@ -6393,35 +6411,35 @@
     </row>
     <row r="16" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="230"/>
-      <c r="B16" s="70">
+      <c r="B16" s="71">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D16" s="70" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="71" t="s">
         <v>166</v>
       </c>
       <c r="E16" s="107">
-        <f>IF(D16="YES",1,0)</f>
-        <v>1</v>
+        <f>IF(D16="YES",0.5,0)</f>
+        <v>0.5</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G16" s="230"/>
     </row>
     <row r="17" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="230"/>
-      <c r="B17" s="70">
+      <c r="B17" s="71">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D17" s="70" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="71" t="s">
         <v>166</v>
       </c>
       <c r="E17" s="107">
@@ -6429,20 +6447,20 @@
         <v>1</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G17" s="230"/>
     </row>
     <row r="18" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="230"/>
-      <c r="B18" s="70">
+      <c r="B18" s="71">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="D18" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="71" t="s">
         <v>166</v>
       </c>
       <c r="E18" s="107">
@@ -6450,41 +6468,41 @@
         <v>1</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="G18" s="230"/>
     </row>
     <row r="19" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="230"/>
-      <c r="B19" s="70">
+      <c r="B19" s="71">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="D19" s="70" t="s">
-        <v>166</v>
+        <v>184</v>
+      </c>
+      <c r="D19" s="71" t="s">
+        <v>143</v>
       </c>
       <c r="E19" s="107">
-        <f>IF(D19="YES",1,0)</f>
+        <f>IF(D19="NO",1,0)</f>
         <v>1</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" s="230"/>
     </row>
     <row r="20" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="230"/>
-      <c r="B20" s="70">
+      <c r="B20" s="71">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" s="70" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="71" t="s">
         <v>166</v>
       </c>
       <c r="E20" s="107">
@@ -6492,41 +6510,39 @@
         <v>1</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="230"/>
     </row>
     <row r="21" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="230"/>
-      <c r="B21" s="70">
+      <c r="B21" s="71">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" s="70" t="s">
-        <v>143</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="D21" s="71"/>
       <c r="E21" s="107">
-        <f>IF(D21="NO",1,0)</f>
-        <v>1</v>
+        <f>IF(D21="YES",1,0)</f>
+        <v>0</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G21" s="230"/>
     </row>
     <row r="22" spans="1:7" s="25" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="230"/>
-      <c r="B22" s="70">
+      <c r="B22" s="71">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="D22" s="70" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" s="71" t="s">
         <v>143</v>
       </c>
       <c r="E22" s="107">
@@ -6534,12 +6550,29 @@
         <v>1</v>
       </c>
       <c r="F22" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="230"/>
+    </row>
+    <row r="23" spans="1:7" ht="18" customHeight="1">
+      <c r="A23" s="230"/>
+      <c r="B23" s="71">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="107">
+        <f>IF(D23="NO",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="230"/>
-    </row>
-    <row r="23" spans="1:7" ht="5" customHeight="1">
-      <c r="A23" s="230"/>
       <c r="G23" s="230"/>
     </row>
     <row r="24" spans="1:7">
@@ -6561,10 +6594,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <ignoredErrors>
-    <ignoredError sqref="E4:E11 E13:E18 E19:E22" emptyCellReference="1"/>
-    <ignoredError sqref="E12" formula="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -9250,7 +9279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7:H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>